<commit_message>
240423 14:50 Update API
</commit_message>
<xml_diff>
--- a/API 명세서.xlsx
+++ b/API 명세서.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="69">
   <si>
     <t>설명</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -354,6 +354,20 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>/email-auth</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>인증 번호를 전송할 유저 이메일 
+(이메일 형태의 데이터)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>curl -v -X POST "http://localhost:4000/api/v1/auth/email-auth \
+  -d "userEmail=email@email.com"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>응답 : 성공
 HTTP/1.1 200 OK
 Content_Type: application/json;charset=UTF-8
@@ -373,7 +387,14 @@
 Content_Type: application/json;charset=UTF-8
 {
   "code": "DE",
-  "message": "Duplicatied email."
+  "message": "Duplicatied Email."
+}
+응답 : 실패 (이메일 전송 실패)
+HTTP/1.1 500 Intermal Server Error
+Content_Type: application/json;charset=UTF-8
+{
+  "code": "MF",
+  "message": "Mai send Failed."
 }
 응답 : 실패 (데이터베이스 오류)
 HTTP/1.1 500 Intermal Server Error
@@ -385,17 +406,33 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>/email-auth</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>인증 번호를 전송할 유저 이메일 
-(이메일 형태의 데이터)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>curl -v -X POST "http://localhost:4000/api/v1/auth/email-auth \
-  -d "userEmail=email@email.com"</t>
+    <t>이메일 인증 확인</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>클라이언트로부터 이메일과 인증 번호를 입력받아 해당하는 이메일에 전송한 인증번호와 일치하는지 확인 합니다. 일치한다면 성공처리를 합니다. 만약 일치하지 않는다면 실패처리를 합니다. 데이터베이스 오류가 발생할 수 있습니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/email-auth-check</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">인증 번호를 확인할 유저 이메일 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>authNumber</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>인증 확인할 인증 번호</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>curl -v -X POST "http://localhost:4000/api/v1/auth/email-auth-check \
+  -d "userEmail=email@email.com" \
+  -d "authNumber=0123"</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1020,6 +1057,18 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1038,18 +1087,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1104,13 +1141,55 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1146,24 +1225,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1215,32 +1276,8 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1522,486 +1559,486 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:L150"/>
+  <dimension ref="B2:L180"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A122" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="N137" sqref="N137"/>
+    <sheetView tabSelected="1" topLeftCell="A178" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="L191" sqref="L191"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="2" spans="2:12" ht="54" x14ac:dyDescent="0.3">
-      <c r="B2" s="52" t="s">
+      <c r="B2" s="60" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="53"/>
-      <c r="D2" s="53"/>
-      <c r="E2" s="53"/>
-      <c r="F2" s="53"/>
-      <c r="G2" s="53"/>
-      <c r="H2" s="53"/>
-      <c r="I2" s="53"/>
-      <c r="J2" s="53"/>
-      <c r="K2" s="54"/>
+      <c r="C2" s="61"/>
+      <c r="D2" s="61"/>
+      <c r="E2" s="61"/>
+      <c r="F2" s="61"/>
+      <c r="G2" s="61"/>
+      <c r="H2" s="61"/>
+      <c r="I2" s="61"/>
+      <c r="J2" s="61"/>
+      <c r="K2" s="62"/>
       <c r="L2" s="1"/>
     </row>
     <row r="3" spans="2:12" ht="31.5" x14ac:dyDescent="0.3">
-      <c r="B3" s="55" t="s">
+      <c r="B3" s="63" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="56"/>
-      <c r="D3" s="56"/>
-      <c r="E3" s="56"/>
-      <c r="F3" s="56"/>
-      <c r="G3" s="56"/>
-      <c r="H3" s="56"/>
-      <c r="I3" s="56"/>
-      <c r="J3" s="56"/>
-      <c r="K3" s="57"/>
+      <c r="C3" s="64"/>
+      <c r="D3" s="64"/>
+      <c r="E3" s="64"/>
+      <c r="F3" s="64"/>
+      <c r="G3" s="64"/>
+      <c r="H3" s="64"/>
+      <c r="I3" s="64"/>
+      <c r="J3" s="64"/>
+      <c r="K3" s="65"/>
       <c r="L3" s="2"/>
     </row>
     <row r="4" spans="2:12" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="58" t="s">
+      <c r="B4" s="66" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="59"/>
-      <c r="D4" s="59"/>
-      <c r="E4" s="59"/>
-      <c r="F4" s="59"/>
-      <c r="G4" s="59"/>
-      <c r="H4" s="59"/>
-      <c r="I4" s="59"/>
-      <c r="J4" s="59"/>
-      <c r="K4" s="60"/>
+      <c r="C4" s="67"/>
+      <c r="D4" s="67"/>
+      <c r="E4" s="67"/>
+      <c r="F4" s="67"/>
+      <c r="G4" s="67"/>
+      <c r="H4" s="67"/>
+      <c r="I4" s="67"/>
+      <c r="J4" s="67"/>
+      <c r="K4" s="68"/>
       <c r="L4" s="3"/>
     </row>
     <row r="5" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="61"/>
-      <c r="C5" s="62"/>
-      <c r="D5" s="62"/>
-      <c r="E5" s="62"/>
-      <c r="F5" s="62"/>
-      <c r="G5" s="62"/>
-      <c r="H5" s="62"/>
-      <c r="I5" s="62"/>
-      <c r="J5" s="62"/>
-      <c r="K5" s="63"/>
+      <c r="B5" s="69"/>
+      <c r="C5" s="70"/>
+      <c r="D5" s="70"/>
+      <c r="E5" s="70"/>
+      <c r="F5" s="70"/>
+      <c r="G5" s="70"/>
+      <c r="H5" s="70"/>
+      <c r="I5" s="70"/>
+      <c r="J5" s="70"/>
+      <c r="K5" s="71"/>
       <c r="L5" s="3"/>
     </row>
     <row r="6" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="61"/>
-      <c r="C6" s="62"/>
-      <c r="D6" s="62"/>
-      <c r="E6" s="62"/>
-      <c r="F6" s="62"/>
-      <c r="G6" s="62"/>
-      <c r="H6" s="62"/>
-      <c r="I6" s="62"/>
-      <c r="J6" s="62"/>
-      <c r="K6" s="63"/>
+      <c r="B6" s="69"/>
+      <c r="C6" s="70"/>
+      <c r="D6" s="70"/>
+      <c r="E6" s="70"/>
+      <c r="F6" s="70"/>
+      <c r="G6" s="70"/>
+      <c r="H6" s="70"/>
+      <c r="I6" s="70"/>
+      <c r="J6" s="70"/>
+      <c r="K6" s="71"/>
       <c r="L6" s="3"/>
     </row>
     <row r="7" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="61"/>
-      <c r="C7" s="62"/>
-      <c r="D7" s="62"/>
-      <c r="E7" s="62"/>
-      <c r="F7" s="62"/>
-      <c r="G7" s="62"/>
-      <c r="H7" s="62"/>
-      <c r="I7" s="62"/>
-      <c r="J7" s="62"/>
-      <c r="K7" s="63"/>
+      <c r="B7" s="69"/>
+      <c r="C7" s="70"/>
+      <c r="D7" s="70"/>
+      <c r="E7" s="70"/>
+      <c r="F7" s="70"/>
+      <c r="G7" s="70"/>
+      <c r="H7" s="70"/>
+      <c r="I7" s="70"/>
+      <c r="J7" s="70"/>
+      <c r="K7" s="71"/>
       <c r="L7" s="3"/>
     </row>
     <row r="8" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="61"/>
-      <c r="C8" s="62"/>
-      <c r="D8" s="62"/>
-      <c r="E8" s="62"/>
-      <c r="F8" s="62"/>
-      <c r="G8" s="62"/>
-      <c r="H8" s="62"/>
-      <c r="I8" s="62"/>
-      <c r="J8" s="62"/>
-      <c r="K8" s="63"/>
+      <c r="B8" s="69"/>
+      <c r="C8" s="70"/>
+      <c r="D8" s="70"/>
+      <c r="E8" s="70"/>
+      <c r="F8" s="70"/>
+      <c r="G8" s="70"/>
+      <c r="H8" s="70"/>
+      <c r="I8" s="70"/>
+      <c r="J8" s="70"/>
+      <c r="K8" s="71"/>
       <c r="L8" s="3"/>
     </row>
     <row r="9" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="61"/>
-      <c r="C9" s="62"/>
-      <c r="D9" s="62"/>
-      <c r="E9" s="62"/>
-      <c r="F9" s="62"/>
-      <c r="G9" s="62"/>
-      <c r="H9" s="62"/>
-      <c r="I9" s="62"/>
-      <c r="J9" s="62"/>
-      <c r="K9" s="63"/>
+      <c r="B9" s="69"/>
+      <c r="C9" s="70"/>
+      <c r="D9" s="70"/>
+      <c r="E9" s="70"/>
+      <c r="F9" s="70"/>
+      <c r="G9" s="70"/>
+      <c r="H9" s="70"/>
+      <c r="I9" s="70"/>
+      <c r="J9" s="70"/>
+      <c r="K9" s="71"/>
       <c r="L9" s="3"/>
     </row>
     <row r="10" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="61"/>
-      <c r="C10" s="62"/>
-      <c r="D10" s="62"/>
-      <c r="E10" s="62"/>
-      <c r="F10" s="62"/>
-      <c r="G10" s="62"/>
-      <c r="H10" s="62"/>
-      <c r="I10" s="62"/>
-      <c r="J10" s="62"/>
-      <c r="K10" s="63"/>
+      <c r="B10" s="69"/>
+      <c r="C10" s="70"/>
+      <c r="D10" s="70"/>
+      <c r="E10" s="70"/>
+      <c r="F10" s="70"/>
+      <c r="G10" s="70"/>
+      <c r="H10" s="70"/>
+      <c r="I10" s="70"/>
+      <c r="J10" s="70"/>
+      <c r="K10" s="71"/>
       <c r="L10" s="3"/>
     </row>
     <row r="11" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="61"/>
-      <c r="C11" s="62"/>
-      <c r="D11" s="62"/>
-      <c r="E11" s="62"/>
-      <c r="F11" s="62"/>
-      <c r="G11" s="62"/>
-      <c r="H11" s="62"/>
-      <c r="I11" s="62"/>
-      <c r="J11" s="62"/>
-      <c r="K11" s="63"/>
+      <c r="B11" s="69"/>
+      <c r="C11" s="70"/>
+      <c r="D11" s="70"/>
+      <c r="E11" s="70"/>
+      <c r="F11" s="70"/>
+      <c r="G11" s="70"/>
+      <c r="H11" s="70"/>
+      <c r="I11" s="70"/>
+      <c r="J11" s="70"/>
+      <c r="K11" s="71"/>
       <c r="L11" s="3"/>
     </row>
     <row r="12" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="61"/>
-      <c r="C12" s="62"/>
-      <c r="D12" s="62"/>
-      <c r="E12" s="62"/>
-      <c r="F12" s="62"/>
-      <c r="G12" s="62"/>
-      <c r="H12" s="62"/>
-      <c r="I12" s="62"/>
-      <c r="J12" s="62"/>
-      <c r="K12" s="63"/>
+      <c r="B12" s="69"/>
+      <c r="C12" s="70"/>
+      <c r="D12" s="70"/>
+      <c r="E12" s="70"/>
+      <c r="F12" s="70"/>
+      <c r="G12" s="70"/>
+      <c r="H12" s="70"/>
+      <c r="I12" s="70"/>
+      <c r="J12" s="70"/>
+      <c r="K12" s="71"/>
       <c r="L12" s="3"/>
     </row>
     <row r="13" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="61"/>
-      <c r="C13" s="62"/>
-      <c r="D13" s="62"/>
-      <c r="E13" s="62"/>
-      <c r="F13" s="62"/>
-      <c r="G13" s="62"/>
-      <c r="H13" s="62"/>
-      <c r="I13" s="62"/>
-      <c r="J13" s="62"/>
-      <c r="K13" s="63"/>
+      <c r="B13" s="69"/>
+      <c r="C13" s="70"/>
+      <c r="D13" s="70"/>
+      <c r="E13" s="70"/>
+      <c r="F13" s="70"/>
+      <c r="G13" s="70"/>
+      <c r="H13" s="70"/>
+      <c r="I13" s="70"/>
+      <c r="J13" s="70"/>
+      <c r="K13" s="71"/>
       <c r="L13" s="3"/>
     </row>
     <row r="14" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="61"/>
-      <c r="C14" s="62"/>
-      <c r="D14" s="62"/>
-      <c r="E14" s="62"/>
-      <c r="F14" s="62"/>
-      <c r="G14" s="62"/>
-      <c r="H14" s="62"/>
-      <c r="I14" s="62"/>
-      <c r="J14" s="62"/>
-      <c r="K14" s="63"/>
+      <c r="B14" s="69"/>
+      <c r="C14" s="70"/>
+      <c r="D14" s="70"/>
+      <c r="E14" s="70"/>
+      <c r="F14" s="70"/>
+      <c r="G14" s="70"/>
+      <c r="H14" s="70"/>
+      <c r="I14" s="70"/>
+      <c r="J14" s="70"/>
+      <c r="K14" s="71"/>
       <c r="L14" s="3"/>
     </row>
     <row r="15" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="61"/>
-      <c r="C15" s="62"/>
-      <c r="D15" s="62"/>
-      <c r="E15" s="62"/>
-      <c r="F15" s="62"/>
-      <c r="G15" s="62"/>
-      <c r="H15" s="62"/>
-      <c r="I15" s="62"/>
-      <c r="J15" s="62"/>
-      <c r="K15" s="63"/>
+      <c r="B15" s="69"/>
+      <c r="C15" s="70"/>
+      <c r="D15" s="70"/>
+      <c r="E15" s="70"/>
+      <c r="F15" s="70"/>
+      <c r="G15" s="70"/>
+      <c r="H15" s="70"/>
+      <c r="I15" s="70"/>
+      <c r="J15" s="70"/>
+      <c r="K15" s="71"/>
       <c r="L15" s="3"/>
     </row>
     <row r="16" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="61"/>
-      <c r="C16" s="62"/>
-      <c r="D16" s="62"/>
-      <c r="E16" s="62"/>
-      <c r="F16" s="62"/>
-      <c r="G16" s="62"/>
-      <c r="H16" s="62"/>
-      <c r="I16" s="62"/>
-      <c r="J16" s="62"/>
-      <c r="K16" s="63"/>
+      <c r="B16" s="69"/>
+      <c r="C16" s="70"/>
+      <c r="D16" s="70"/>
+      <c r="E16" s="70"/>
+      <c r="F16" s="70"/>
+      <c r="G16" s="70"/>
+      <c r="H16" s="70"/>
+      <c r="I16" s="70"/>
+      <c r="J16" s="70"/>
+      <c r="K16" s="71"/>
       <c r="L16" s="3"/>
     </row>
     <row r="17" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="61"/>
-      <c r="C17" s="62"/>
-      <c r="D17" s="62"/>
-      <c r="E17" s="62"/>
-      <c r="F17" s="62"/>
-      <c r="G17" s="62"/>
-      <c r="H17" s="62"/>
-      <c r="I17" s="62"/>
-      <c r="J17" s="62"/>
-      <c r="K17" s="63"/>
+      <c r="B17" s="69"/>
+      <c r="C17" s="70"/>
+      <c r="D17" s="70"/>
+      <c r="E17" s="70"/>
+      <c r="F17" s="70"/>
+      <c r="G17" s="70"/>
+      <c r="H17" s="70"/>
+      <c r="I17" s="70"/>
+      <c r="J17" s="70"/>
+      <c r="K17" s="71"/>
       <c r="L17" s="3"/>
     </row>
     <row r="18" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="61"/>
-      <c r="C18" s="62"/>
-      <c r="D18" s="62"/>
-      <c r="E18" s="62"/>
-      <c r="F18" s="62"/>
-      <c r="G18" s="62"/>
-      <c r="H18" s="62"/>
-      <c r="I18" s="62"/>
-      <c r="J18" s="62"/>
-      <c r="K18" s="63"/>
+      <c r="B18" s="69"/>
+      <c r="C18" s="70"/>
+      <c r="D18" s="70"/>
+      <c r="E18" s="70"/>
+      <c r="F18" s="70"/>
+      <c r="G18" s="70"/>
+      <c r="H18" s="70"/>
+      <c r="I18" s="70"/>
+      <c r="J18" s="70"/>
+      <c r="K18" s="71"/>
       <c r="L18" s="3"/>
     </row>
     <row r="19" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="61"/>
-      <c r="C19" s="62"/>
-      <c r="D19" s="62"/>
-      <c r="E19" s="62"/>
-      <c r="F19" s="62"/>
-      <c r="G19" s="62"/>
-      <c r="H19" s="62"/>
-      <c r="I19" s="62"/>
-      <c r="J19" s="62"/>
-      <c r="K19" s="63"/>
+      <c r="B19" s="69"/>
+      <c r="C19" s="70"/>
+      <c r="D19" s="70"/>
+      <c r="E19" s="70"/>
+      <c r="F19" s="70"/>
+      <c r="G19" s="70"/>
+      <c r="H19" s="70"/>
+      <c r="I19" s="70"/>
+      <c r="J19" s="70"/>
+      <c r="K19" s="71"/>
       <c r="L19" s="3"/>
     </row>
     <row r="20" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="61"/>
-      <c r="C20" s="62"/>
-      <c r="D20" s="62"/>
-      <c r="E20" s="62"/>
-      <c r="F20" s="62"/>
-      <c r="G20" s="62"/>
-      <c r="H20" s="62"/>
-      <c r="I20" s="62"/>
-      <c r="J20" s="62"/>
-      <c r="K20" s="63"/>
+      <c r="B20" s="69"/>
+      <c r="C20" s="70"/>
+      <c r="D20" s="70"/>
+      <c r="E20" s="70"/>
+      <c r="F20" s="70"/>
+      <c r="G20" s="70"/>
+      <c r="H20" s="70"/>
+      <c r="I20" s="70"/>
+      <c r="J20" s="70"/>
+      <c r="K20" s="71"/>
       <c r="L20" s="3"/>
     </row>
     <row r="21" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="61"/>
-      <c r="C21" s="62"/>
-      <c r="D21" s="62"/>
-      <c r="E21" s="62"/>
-      <c r="F21" s="62"/>
-      <c r="G21" s="62"/>
-      <c r="H21" s="62"/>
-      <c r="I21" s="62"/>
-      <c r="J21" s="62"/>
-      <c r="K21" s="63"/>
+      <c r="B21" s="69"/>
+      <c r="C21" s="70"/>
+      <c r="D21" s="70"/>
+      <c r="E21" s="70"/>
+      <c r="F21" s="70"/>
+      <c r="G21" s="70"/>
+      <c r="H21" s="70"/>
+      <c r="I21" s="70"/>
+      <c r="J21" s="70"/>
+      <c r="K21" s="71"/>
       <c r="L21" s="3"/>
     </row>
     <row r="22" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="61"/>
-      <c r="C22" s="62"/>
-      <c r="D22" s="62"/>
-      <c r="E22" s="62"/>
-      <c r="F22" s="62"/>
-      <c r="G22" s="62"/>
-      <c r="H22" s="62"/>
-      <c r="I22" s="62"/>
-      <c r="J22" s="62"/>
-      <c r="K22" s="63"/>
+      <c r="B22" s="69"/>
+      <c r="C22" s="70"/>
+      <c r="D22" s="70"/>
+      <c r="E22" s="70"/>
+      <c r="F22" s="70"/>
+      <c r="G22" s="70"/>
+      <c r="H22" s="70"/>
+      <c r="I22" s="70"/>
+      <c r="J22" s="70"/>
+      <c r="K22" s="71"/>
       <c r="L22" s="3"/>
     </row>
     <row r="23" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="61"/>
-      <c r="C23" s="62"/>
-      <c r="D23" s="62"/>
-      <c r="E23" s="62"/>
-      <c r="F23" s="62"/>
-      <c r="G23" s="62"/>
-      <c r="H23" s="62"/>
-      <c r="I23" s="62"/>
-      <c r="J23" s="62"/>
-      <c r="K23" s="63"/>
+      <c r="B23" s="69"/>
+      <c r="C23" s="70"/>
+      <c r="D23" s="70"/>
+      <c r="E23" s="70"/>
+      <c r="F23" s="70"/>
+      <c r="G23" s="70"/>
+      <c r="H23" s="70"/>
+      <c r="I23" s="70"/>
+      <c r="J23" s="70"/>
+      <c r="K23" s="71"/>
       <c r="L23" s="3"/>
     </row>
     <row r="24" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="61"/>
-      <c r="C24" s="62"/>
-      <c r="D24" s="62"/>
-      <c r="E24" s="62"/>
-      <c r="F24" s="62"/>
-      <c r="G24" s="62"/>
-      <c r="H24" s="62"/>
-      <c r="I24" s="62"/>
-      <c r="J24" s="62"/>
-      <c r="K24" s="63"/>
+      <c r="B24" s="69"/>
+      <c r="C24" s="70"/>
+      <c r="D24" s="70"/>
+      <c r="E24" s="70"/>
+      <c r="F24" s="70"/>
+      <c r="G24" s="70"/>
+      <c r="H24" s="70"/>
+      <c r="I24" s="70"/>
+      <c r="J24" s="70"/>
+      <c r="K24" s="71"/>
       <c r="L24" s="3"/>
     </row>
     <row r="25" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="61"/>
-      <c r="C25" s="62"/>
-      <c r="D25" s="62"/>
-      <c r="E25" s="62"/>
-      <c r="F25" s="62"/>
-      <c r="G25" s="62"/>
-      <c r="H25" s="62"/>
-      <c r="I25" s="62"/>
-      <c r="J25" s="62"/>
-      <c r="K25" s="63"/>
+      <c r="B25" s="69"/>
+      <c r="C25" s="70"/>
+      <c r="D25" s="70"/>
+      <c r="E25" s="70"/>
+      <c r="F25" s="70"/>
+      <c r="G25" s="70"/>
+      <c r="H25" s="70"/>
+      <c r="I25" s="70"/>
+      <c r="J25" s="70"/>
+      <c r="K25" s="71"/>
       <c r="L25" s="3"/>
     </row>
     <row r="26" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="61"/>
-      <c r="C26" s="62"/>
-      <c r="D26" s="62"/>
-      <c r="E26" s="62"/>
-      <c r="F26" s="62"/>
-      <c r="G26" s="62"/>
-      <c r="H26" s="62"/>
-      <c r="I26" s="62"/>
-      <c r="J26" s="62"/>
-      <c r="K26" s="63"/>
+      <c r="B26" s="69"/>
+      <c r="C26" s="70"/>
+      <c r="D26" s="70"/>
+      <c r="E26" s="70"/>
+      <c r="F26" s="70"/>
+      <c r="G26" s="70"/>
+      <c r="H26" s="70"/>
+      <c r="I26" s="70"/>
+      <c r="J26" s="70"/>
+      <c r="K26" s="71"/>
       <c r="L26" s="3"/>
     </row>
     <row r="27" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="61"/>
-      <c r="C27" s="62"/>
-      <c r="D27" s="62"/>
-      <c r="E27" s="62"/>
-      <c r="F27" s="62"/>
-      <c r="G27" s="62"/>
-      <c r="H27" s="62"/>
-      <c r="I27" s="62"/>
-      <c r="J27" s="62"/>
-      <c r="K27" s="63"/>
+      <c r="B27" s="69"/>
+      <c r="C27" s="70"/>
+      <c r="D27" s="70"/>
+      <c r="E27" s="70"/>
+      <c r="F27" s="70"/>
+      <c r="G27" s="70"/>
+      <c r="H27" s="70"/>
+      <c r="I27" s="70"/>
+      <c r="J27" s="70"/>
+      <c r="K27" s="71"/>
       <c r="L27" s="3"/>
     </row>
     <row r="28" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="64"/>
-      <c r="C28" s="65"/>
-      <c r="D28" s="65"/>
-      <c r="E28" s="65"/>
-      <c r="F28" s="65"/>
-      <c r="G28" s="65"/>
-      <c r="H28" s="65"/>
-      <c r="I28" s="65"/>
-      <c r="J28" s="65"/>
-      <c r="K28" s="66"/>
+      <c r="B28" s="72"/>
+      <c r="C28" s="73"/>
+      <c r="D28" s="73"/>
+      <c r="E28" s="73"/>
+      <c r="F28" s="73"/>
+      <c r="G28" s="73"/>
+      <c r="H28" s="73"/>
+      <c r="I28" s="73"/>
+      <c r="J28" s="73"/>
+      <c r="K28" s="74"/>
       <c r="L28" s="3"/>
     </row>
     <row r="29" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="39" t="s">
+      <c r="B29" s="53" t="s">
         <v>5</v>
       </c>
-      <c r="C29" s="39"/>
-      <c r="D29" s="39"/>
-      <c r="E29" s="67" t="s">
+      <c r="C29" s="53"/>
+      <c r="D29" s="53"/>
+      <c r="E29" s="75" t="s">
         <v>20</v>
       </c>
-      <c r="F29" s="67"/>
-      <c r="G29" s="67"/>
-      <c r="H29" s="67"/>
-      <c r="I29" s="67"/>
-      <c r="J29" s="67"/>
-      <c r="K29" s="68"/>
+      <c r="F29" s="75"/>
+      <c r="G29" s="75"/>
+      <c r="H29" s="75"/>
+      <c r="I29" s="75"/>
+      <c r="J29" s="75"/>
+      <c r="K29" s="76"/>
       <c r="L29" s="3"/>
     </row>
     <row r="30" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="31" spans="2:12" ht="41.25" x14ac:dyDescent="0.3">
-      <c r="B31" s="35" t="s">
+      <c r="B31" s="49" t="s">
         <v>17</v>
       </c>
-      <c r="C31" s="36"/>
-      <c r="D31" s="36"/>
-      <c r="E31" s="36"/>
-      <c r="F31" s="36"/>
-      <c r="G31" s="36"/>
-      <c r="H31" s="36"/>
-      <c r="I31" s="36"/>
-      <c r="J31" s="36"/>
-      <c r="K31" s="37"/>
+      <c r="C31" s="50"/>
+      <c r="D31" s="50"/>
+      <c r="E31" s="50"/>
+      <c r="F31" s="50"/>
+      <c r="G31" s="50"/>
+      <c r="H31" s="50"/>
+      <c r="I31" s="50"/>
+      <c r="J31" s="50"/>
+      <c r="K31" s="51"/>
     </row>
     <row r="32" spans="2:12" ht="26.25" x14ac:dyDescent="0.3">
-      <c r="B32" s="38" t="s">
+      <c r="B32" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="C32" s="39"/>
-      <c r="D32" s="39"/>
-      <c r="E32" s="39"/>
-      <c r="F32" s="39"/>
-      <c r="G32" s="39"/>
-      <c r="H32" s="39"/>
-      <c r="I32" s="39"/>
-      <c r="J32" s="39"/>
-      <c r="K32" s="40"/>
+      <c r="C32" s="53"/>
+      <c r="D32" s="53"/>
+      <c r="E32" s="53"/>
+      <c r="F32" s="53"/>
+      <c r="G32" s="53"/>
+      <c r="H32" s="53"/>
+      <c r="I32" s="53"/>
+      <c r="J32" s="53"/>
+      <c r="K32" s="54"/>
     </row>
     <row r="33" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B33" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="C33" s="41"/>
-      <c r="D33" s="41"/>
-      <c r="E33" s="41"/>
-      <c r="F33" s="41"/>
-      <c r="G33" s="41"/>
-      <c r="H33" s="41"/>
-      <c r="I33" s="41"/>
-      <c r="J33" s="41"/>
-      <c r="K33" s="42"/>
+      <c r="C33" s="55"/>
+      <c r="D33" s="55"/>
+      <c r="E33" s="55"/>
+      <c r="F33" s="55"/>
+      <c r="G33" s="55"/>
+      <c r="H33" s="55"/>
+      <c r="I33" s="55"/>
+      <c r="J33" s="55"/>
+      <c r="K33" s="56"/>
     </row>
     <row r="34" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B34" s="19"/>
-      <c r="C34" s="41"/>
-      <c r="D34" s="41"/>
-      <c r="E34" s="41"/>
-      <c r="F34" s="41"/>
-      <c r="G34" s="41"/>
-      <c r="H34" s="41"/>
-      <c r="I34" s="41"/>
-      <c r="J34" s="41"/>
-      <c r="K34" s="42"/>
+      <c r="C34" s="55"/>
+      <c r="D34" s="55"/>
+      <c r="E34" s="55"/>
+      <c r="F34" s="55"/>
+      <c r="G34" s="55"/>
+      <c r="H34" s="55"/>
+      <c r="I34" s="55"/>
+      <c r="J34" s="55"/>
+      <c r="K34" s="56"/>
     </row>
     <row r="35" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B35" s="19"/>
-      <c r="C35" s="41"/>
-      <c r="D35" s="41"/>
-      <c r="E35" s="41"/>
-      <c r="F35" s="41"/>
-      <c r="G35" s="41"/>
-      <c r="H35" s="41"/>
-      <c r="I35" s="41"/>
-      <c r="J35" s="41"/>
-      <c r="K35" s="42"/>
+      <c r="C35" s="55"/>
+      <c r="D35" s="55"/>
+      <c r="E35" s="55"/>
+      <c r="F35" s="55"/>
+      <c r="G35" s="55"/>
+      <c r="H35" s="55"/>
+      <c r="I35" s="55"/>
+      <c r="J35" s="55"/>
+      <c r="K35" s="56"/>
     </row>
     <row r="36" spans="2:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B36" s="43"/>
-      <c r="C36" s="44"/>
-      <c r="D36" s="44"/>
-      <c r="E36" s="44"/>
-      <c r="F36" s="44"/>
-      <c r="G36" s="44"/>
-      <c r="H36" s="44"/>
-      <c r="I36" s="44"/>
-      <c r="J36" s="44"/>
-      <c r="K36" s="45"/>
+      <c r="B36" s="57"/>
+      <c r="C36" s="58"/>
+      <c r="D36" s="58"/>
+      <c r="E36" s="58"/>
+      <c r="F36" s="58"/>
+      <c r="G36" s="58"/>
+      <c r="H36" s="58"/>
+      <c r="I36" s="58"/>
+      <c r="J36" s="58"/>
+      <c r="K36" s="59"/>
     </row>
     <row r="37" spans="2:11" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B37" s="26" t="s">
         <v>4</v>
       </c>
       <c r="C37" s="27"/>
-      <c r="D37" s="46" t="s">
+      <c r="D37" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="E37" s="46"/>
-      <c r="F37" s="47"/>
-      <c r="G37" s="48" t="s">
+      <c r="E37" s="36"/>
+      <c r="F37" s="37"/>
+      <c r="G37" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="H37" s="49"/>
-      <c r="I37" s="50" t="s">
+      <c r="H37" s="39"/>
+      <c r="I37" s="40" t="s">
         <v>21</v>
       </c>
-      <c r="J37" s="50"/>
-      <c r="K37" s="51"/>
+      <c r="J37" s="40"/>
+      <c r="K37" s="41"/>
     </row>
     <row r="38" spans="2:11" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B38" s="26" t="s">
@@ -2021,15 +2058,15 @@
       <c r="B39" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="C39" s="33"/>
-      <c r="D39" s="33"/>
-      <c r="E39" s="33"/>
-      <c r="F39" s="33"/>
-      <c r="G39" s="33"/>
-      <c r="H39" s="33"/>
-      <c r="I39" s="33"/>
-      <c r="J39" s="33"/>
-      <c r="K39" s="34"/>
+      <c r="C39" s="42"/>
+      <c r="D39" s="42"/>
+      <c r="E39" s="42"/>
+      <c r="F39" s="42"/>
+      <c r="G39" s="42"/>
+      <c r="H39" s="42"/>
+      <c r="I39" s="42"/>
+      <c r="J39" s="42"/>
+      <c r="K39" s="43"/>
     </row>
     <row r="40" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B40" s="14" t="s">
@@ -2050,19 +2087,19 @@
       <c r="K40" s="16"/>
     </row>
     <row r="41" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B41" s="10"/>
-      <c r="C41" s="11"/>
-      <c r="D41" s="11"/>
-      <c r="E41" s="11"/>
-      <c r="F41" s="11"/>
-      <c r="G41" s="11"/>
-      <c r="H41" s="11"/>
-      <c r="I41" s="11"/>
-      <c r="J41" s="11"/>
-      <c r="K41" s="13"/>
+      <c r="B41" s="4"/>
+      <c r="C41" s="5"/>
+      <c r="D41" s="5"/>
+      <c r="E41" s="5"/>
+      <c r="F41" s="5"/>
+      <c r="G41" s="5"/>
+      <c r="H41" s="5"/>
+      <c r="I41" s="5"/>
+      <c r="J41" s="5"/>
+      <c r="K41" s="7"/>
     </row>
     <row r="42" spans="2:11" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="B42" s="4" t="s">
+      <c r="B42" s="8" t="s">
         <v>11</v>
       </c>
       <c r="C42" s="17"/>
@@ -2096,47 +2133,47 @@
       <c r="K43" s="16"/>
     </row>
     <row r="44" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B44" s="10" t="s">
+      <c r="B44" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C44" s="11"/>
-      <c r="D44" s="11" t="s">
+      <c r="C44" s="5"/>
+      <c r="D44" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E44" s="32"/>
-      <c r="F44" s="11" t="s">
+      <c r="E44" s="77"/>
+      <c r="F44" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="G44" s="11"/>
-      <c r="H44" s="11"/>
-      <c r="I44" s="11"/>
-      <c r="J44" s="12" t="s">
+      <c r="G44" s="5"/>
+      <c r="H44" s="5"/>
+      <c r="I44" s="5"/>
+      <c r="J44" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="K44" s="13"/>
+      <c r="K44" s="7"/>
     </row>
     <row r="45" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B45" s="10" t="s">
+      <c r="B45" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C45" s="11"/>
-      <c r="D45" s="11" t="s">
+      <c r="C45" s="5"/>
+      <c r="D45" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E45" s="11"/>
-      <c r="F45" s="11" t="s">
+      <c r="E45" s="5"/>
+      <c r="F45" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="G45" s="11"/>
-      <c r="H45" s="11"/>
-      <c r="I45" s="11"/>
-      <c r="J45" s="12" t="s">
+      <c r="G45" s="5"/>
+      <c r="H45" s="5"/>
+      <c r="I45" s="5"/>
+      <c r="J45" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="K45" s="13"/>
+      <c r="K45" s="7"/>
     </row>
     <row r="46" spans="2:11" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="B46" s="4" t="s">
+      <c r="B46" s="8" t="s">
         <v>10</v>
       </c>
       <c r="C46" s="17"/>
@@ -2246,36 +2283,36 @@
       <c r="K53" s="16"/>
     </row>
     <row r="54" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B54" s="10" t="s">
+      <c r="B54" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C54" s="11"/>
-      <c r="D54" s="11" t="s">
+      <c r="C54" s="5"/>
+      <c r="D54" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="E54" s="11"/>
-      <c r="F54" s="11"/>
-      <c r="G54" s="11"/>
-      <c r="H54" s="11"/>
-      <c r="I54" s="11"/>
-      <c r="J54" s="12" t="s">
+      <c r="E54" s="5"/>
+      <c r="F54" s="5"/>
+      <c r="G54" s="5"/>
+      <c r="H54" s="5"/>
+      <c r="I54" s="5"/>
+      <c r="J54" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="K54" s="13"/>
+      <c r="K54" s="7"/>
     </row>
     <row r="55" spans="2:11" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="B55" s="4" t="s">
+      <c r="B55" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C55" s="5"/>
-      <c r="D55" s="5"/>
-      <c r="E55" s="5"/>
-      <c r="F55" s="5"/>
-      <c r="G55" s="5"/>
-      <c r="H55" s="5"/>
-      <c r="I55" s="5"/>
-      <c r="J55" s="5"/>
-      <c r="K55" s="6"/>
+      <c r="C55" s="9"/>
+      <c r="D55" s="9"/>
+      <c r="E55" s="9"/>
+      <c r="F55" s="9"/>
+      <c r="G55" s="9"/>
+      <c r="H55" s="9"/>
+      <c r="I55" s="9"/>
+      <c r="J55" s="9"/>
+      <c r="K55" s="10"/>
     </row>
     <row r="56" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B56" s="14" t="s">
@@ -2298,211 +2335,211 @@
       <c r="K56" s="16"/>
     </row>
     <row r="57" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B57" s="10" t="s">
+      <c r="B57" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C57" s="11"/>
-      <c r="D57" s="11" t="s">
+      <c r="C57" s="5"/>
+      <c r="D57" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E57" s="11"/>
-      <c r="F57" s="11" t="s">
+      <c r="E57" s="5"/>
+      <c r="F57" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="G57" s="11"/>
-      <c r="H57" s="11"/>
-      <c r="I57" s="11"/>
-      <c r="J57" s="12" t="s">
+      <c r="G57" s="5"/>
+      <c r="H57" s="5"/>
+      <c r="I57" s="5"/>
+      <c r="J57" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="K57" s="13"/>
+      <c r="K57" s="7"/>
     </row>
     <row r="58" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B58" s="10" t="s">
+      <c r="B58" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C58" s="11"/>
-      <c r="D58" s="11" t="s">
+      <c r="C58" s="5"/>
+      <c r="D58" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E58" s="11"/>
-      <c r="F58" s="11" t="s">
+      <c r="E58" s="5"/>
+      <c r="F58" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="G58" s="11"/>
-      <c r="H58" s="11"/>
-      <c r="I58" s="11"/>
-      <c r="J58" s="12" t="s">
+      <c r="G58" s="5"/>
+      <c r="H58" s="5"/>
+      <c r="I58" s="5"/>
+      <c r="J58" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="K58" s="13"/>
+      <c r="K58" s="7"/>
     </row>
     <row r="59" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B59" s="10" t="s">
+      <c r="B59" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C59" s="11"/>
-      <c r="D59" s="11" t="s">
+      <c r="C59" s="5"/>
+      <c r="D59" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E59" s="11"/>
-      <c r="F59" s="11" t="s">
+      <c r="E59" s="5"/>
+      <c r="F59" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="G59" s="11"/>
-      <c r="H59" s="11"/>
-      <c r="I59" s="11"/>
-      <c r="J59" s="12" t="s">
+      <c r="G59" s="5"/>
+      <c r="H59" s="5"/>
+      <c r="I59" s="5"/>
+      <c r="J59" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="K59" s="13"/>
+      <c r="K59" s="7"/>
     </row>
     <row r="60" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B60" s="10" t="s">
+      <c r="B60" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C60" s="11"/>
-      <c r="D60" s="11" t="s">
+      <c r="C60" s="5"/>
+      <c r="D60" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="E60" s="11"/>
-      <c r="F60" s="11" t="s">
+      <c r="E60" s="5"/>
+      <c r="F60" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="G60" s="11"/>
-      <c r="H60" s="11"/>
-      <c r="I60" s="11"/>
-      <c r="J60" s="12" t="s">
+      <c r="G60" s="5"/>
+      <c r="H60" s="5"/>
+      <c r="I60" s="5"/>
+      <c r="J60" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="K60" s="13"/>
+      <c r="K60" s="7"/>
     </row>
     <row r="61" spans="2:11" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="B61" s="4" t="s">
+      <c r="B61" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C61" s="5"/>
-      <c r="D61" s="5"/>
-      <c r="E61" s="5"/>
-      <c r="F61" s="5"/>
-      <c r="G61" s="5"/>
-      <c r="H61" s="5"/>
-      <c r="I61" s="5"/>
-      <c r="J61" s="5"/>
-      <c r="K61" s="6"/>
+      <c r="C61" s="9"/>
+      <c r="D61" s="9"/>
+      <c r="E61" s="9"/>
+      <c r="F61" s="9"/>
+      <c r="G61" s="9"/>
+      <c r="H61" s="9"/>
+      <c r="I61" s="9"/>
+      <c r="J61" s="9"/>
+      <c r="K61" s="10"/>
     </row>
     <row r="62" spans="2:11" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B62" s="7" t="s">
+      <c r="B62" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="C62" s="8"/>
-      <c r="D62" s="8"/>
-      <c r="E62" s="8"/>
-      <c r="F62" s="8"/>
-      <c r="G62" s="8"/>
-      <c r="H62" s="8"/>
-      <c r="I62" s="8"/>
-      <c r="J62" s="8"/>
-      <c r="K62" s="9"/>
+      <c r="C62" s="12"/>
+      <c r="D62" s="12"/>
+      <c r="E62" s="12"/>
+      <c r="F62" s="12"/>
+      <c r="G62" s="12"/>
+      <c r="H62" s="12"/>
+      <c r="I62" s="12"/>
+      <c r="J62" s="12"/>
+      <c r="K62" s="13"/>
     </row>
     <row r="63" spans="2:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="64" spans="2:11" ht="41.25" x14ac:dyDescent="0.3">
-      <c r="B64" s="35" t="s">
+      <c r="B64" s="49" t="s">
         <v>39</v>
       </c>
-      <c r="C64" s="36"/>
-      <c r="D64" s="36"/>
-      <c r="E64" s="36"/>
-      <c r="F64" s="36"/>
-      <c r="G64" s="36"/>
-      <c r="H64" s="36"/>
-      <c r="I64" s="36"/>
-      <c r="J64" s="36"/>
-      <c r="K64" s="37"/>
+      <c r="C64" s="50"/>
+      <c r="D64" s="50"/>
+      <c r="E64" s="50"/>
+      <c r="F64" s="50"/>
+      <c r="G64" s="50"/>
+      <c r="H64" s="50"/>
+      <c r="I64" s="50"/>
+      <c r="J64" s="50"/>
+      <c r="K64" s="51"/>
     </row>
     <row r="65" spans="2:11" ht="26.25" x14ac:dyDescent="0.3">
-      <c r="B65" s="38" t="s">
+      <c r="B65" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="C65" s="39"/>
-      <c r="D65" s="39"/>
-      <c r="E65" s="39"/>
-      <c r="F65" s="39"/>
-      <c r="G65" s="39"/>
-      <c r="H65" s="39"/>
-      <c r="I65" s="39"/>
-      <c r="J65" s="39"/>
-      <c r="K65" s="40"/>
+      <c r="C65" s="53"/>
+      <c r="D65" s="53"/>
+      <c r="E65" s="53"/>
+      <c r="F65" s="53"/>
+      <c r="G65" s="53"/>
+      <c r="H65" s="53"/>
+      <c r="I65" s="53"/>
+      <c r="J65" s="53"/>
+      <c r="K65" s="54"/>
     </row>
     <row r="66" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B66" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="C66" s="41"/>
-      <c r="D66" s="41"/>
-      <c r="E66" s="41"/>
-      <c r="F66" s="41"/>
-      <c r="G66" s="41"/>
-      <c r="H66" s="41"/>
-      <c r="I66" s="41"/>
-      <c r="J66" s="41"/>
-      <c r="K66" s="42"/>
+      <c r="C66" s="55"/>
+      <c r="D66" s="55"/>
+      <c r="E66" s="55"/>
+      <c r="F66" s="55"/>
+      <c r="G66" s="55"/>
+      <c r="H66" s="55"/>
+      <c r="I66" s="55"/>
+      <c r="J66" s="55"/>
+      <c r="K66" s="56"/>
     </row>
     <row r="67" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B67" s="19"/>
-      <c r="C67" s="41"/>
-      <c r="D67" s="41"/>
-      <c r="E67" s="41"/>
-      <c r="F67" s="41"/>
-      <c r="G67" s="41"/>
-      <c r="H67" s="41"/>
-      <c r="I67" s="41"/>
-      <c r="J67" s="41"/>
-      <c r="K67" s="42"/>
+      <c r="C67" s="55"/>
+      <c r="D67" s="55"/>
+      <c r="E67" s="55"/>
+      <c r="F67" s="55"/>
+      <c r="G67" s="55"/>
+      <c r="H67" s="55"/>
+      <c r="I67" s="55"/>
+      <c r="J67" s="55"/>
+      <c r="K67" s="56"/>
     </row>
     <row r="68" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B68" s="19"/>
-      <c r="C68" s="41"/>
-      <c r="D68" s="41"/>
-      <c r="E68" s="41"/>
-      <c r="F68" s="41"/>
-      <c r="G68" s="41"/>
-      <c r="H68" s="41"/>
-      <c r="I68" s="41"/>
-      <c r="J68" s="41"/>
-      <c r="K68" s="42"/>
+      <c r="C68" s="55"/>
+      <c r="D68" s="55"/>
+      <c r="E68" s="55"/>
+      <c r="F68" s="55"/>
+      <c r="G68" s="55"/>
+      <c r="H68" s="55"/>
+      <c r="I68" s="55"/>
+      <c r="J68" s="55"/>
+      <c r="K68" s="56"/>
     </row>
     <row r="69" spans="2:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B69" s="43"/>
-      <c r="C69" s="44"/>
-      <c r="D69" s="44"/>
-      <c r="E69" s="44"/>
-      <c r="F69" s="44"/>
-      <c r="G69" s="44"/>
-      <c r="H69" s="44"/>
-      <c r="I69" s="44"/>
-      <c r="J69" s="44"/>
-      <c r="K69" s="45"/>
+      <c r="B69" s="57"/>
+      <c r="C69" s="58"/>
+      <c r="D69" s="58"/>
+      <c r="E69" s="58"/>
+      <c r="F69" s="58"/>
+      <c r="G69" s="58"/>
+      <c r="H69" s="58"/>
+      <c r="I69" s="58"/>
+      <c r="J69" s="58"/>
+      <c r="K69" s="59"/>
     </row>
     <row r="70" spans="2:11" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B70" s="26" t="s">
         <v>4</v>
       </c>
       <c r="C70" s="27"/>
-      <c r="D70" s="46" t="s">
+      <c r="D70" s="36" t="s">
         <v>41</v>
       </c>
-      <c r="E70" s="46"/>
-      <c r="F70" s="47"/>
-      <c r="G70" s="48" t="s">
+      <c r="E70" s="36"/>
+      <c r="F70" s="37"/>
+      <c r="G70" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="H70" s="49"/>
-      <c r="I70" s="50" t="s">
+      <c r="H70" s="39"/>
+      <c r="I70" s="40" t="s">
         <v>42</v>
       </c>
-      <c r="J70" s="50"/>
-      <c r="K70" s="51"/>
+      <c r="J70" s="40"/>
+      <c r="K70" s="41"/>
     </row>
     <row r="71" spans="2:11" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B71" s="26" t="s">
@@ -2522,36 +2559,36 @@
       <c r="B72" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="C72" s="33"/>
-      <c r="D72" s="33"/>
-      <c r="E72" s="33"/>
-      <c r="F72" s="33"/>
-      <c r="G72" s="33"/>
-      <c r="H72" s="33"/>
-      <c r="I72" s="33"/>
-      <c r="J72" s="33"/>
-      <c r="K72" s="34"/>
+      <c r="C72" s="42"/>
+      <c r="D72" s="42"/>
+      <c r="E72" s="42"/>
+      <c r="F72" s="42"/>
+      <c r="G72" s="42"/>
+      <c r="H72" s="42"/>
+      <c r="I72" s="42"/>
+      <c r="J72" s="42"/>
+      <c r="K72" s="43"/>
     </row>
     <row r="73" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B73" s="73" t="s">
+      <c r="B73" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="C73" s="72"/>
-      <c r="D73" s="69" t="s">
+      <c r="C73" s="45"/>
+      <c r="D73" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="E73" s="71"/>
-      <c r="F73" s="71"/>
-      <c r="G73" s="71"/>
-      <c r="H73" s="71"/>
-      <c r="I73" s="72"/>
-      <c r="J73" s="69" t="s">
+      <c r="E73" s="47"/>
+      <c r="F73" s="47"/>
+      <c r="G73" s="47"/>
+      <c r="H73" s="47"/>
+      <c r="I73" s="45"/>
+      <c r="J73" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="K73" s="70"/>
+      <c r="K73" s="48"/>
     </row>
     <row r="74" spans="2:11" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="B74" s="4" t="s">
+      <c r="B74" s="8" t="s">
         <v>11</v>
       </c>
       <c r="C74" s="17"/>
@@ -2585,7 +2622,7 @@
       <c r="K75" s="16"/>
     </row>
     <row r="76" spans="2:11" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="B76" s="4" t="s">
+      <c r="B76" s="8" t="s">
         <v>10</v>
       </c>
       <c r="C76" s="17"/>
@@ -2695,36 +2732,36 @@
       <c r="K83" s="16"/>
     </row>
     <row r="84" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B84" s="10" t="s">
+      <c r="B84" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C84" s="11"/>
-      <c r="D84" s="11" t="s">
+      <c r="C84" s="5"/>
+      <c r="D84" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="E84" s="11"/>
-      <c r="F84" s="11"/>
-      <c r="G84" s="11"/>
-      <c r="H84" s="11"/>
-      <c r="I84" s="11"/>
-      <c r="J84" s="12" t="s">
+      <c r="E84" s="5"/>
+      <c r="F84" s="5"/>
+      <c r="G84" s="5"/>
+      <c r="H84" s="5"/>
+      <c r="I84" s="5"/>
+      <c r="J84" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="K84" s="13"/>
+      <c r="K84" s="7"/>
     </row>
     <row r="85" spans="2:11" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="B85" s="4" t="s">
+      <c r="B85" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C85" s="5"/>
-      <c r="D85" s="5"/>
-      <c r="E85" s="5"/>
-      <c r="F85" s="5"/>
-      <c r="G85" s="5"/>
-      <c r="H85" s="5"/>
-      <c r="I85" s="5"/>
-      <c r="J85" s="5"/>
-      <c r="K85" s="6"/>
+      <c r="C85" s="9"/>
+      <c r="D85" s="9"/>
+      <c r="E85" s="9"/>
+      <c r="F85" s="9"/>
+      <c r="G85" s="9"/>
+      <c r="H85" s="9"/>
+      <c r="I85" s="9"/>
+      <c r="J85" s="9"/>
+      <c r="K85" s="10"/>
     </row>
     <row r="86" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B86" s="14" t="s">
@@ -2747,211 +2784,211 @@
       <c r="K86" s="16"/>
     </row>
     <row r="87" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B87" s="10" t="s">
+      <c r="B87" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C87" s="11"/>
-      <c r="D87" s="11" t="s">
+      <c r="C87" s="5"/>
+      <c r="D87" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E87" s="11"/>
-      <c r="F87" s="11" t="s">
+      <c r="E87" s="5"/>
+      <c r="F87" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="G87" s="11"/>
-      <c r="H87" s="11"/>
-      <c r="I87" s="11"/>
-      <c r="J87" s="12" t="s">
+      <c r="G87" s="5"/>
+      <c r="H87" s="5"/>
+      <c r="I87" s="5"/>
+      <c r="J87" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="K87" s="13"/>
+      <c r="K87" s="7"/>
     </row>
     <row r="88" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B88" s="10" t="s">
+      <c r="B88" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C88" s="11"/>
-      <c r="D88" s="11" t="s">
+      <c r="C88" s="5"/>
+      <c r="D88" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E88" s="11"/>
-      <c r="F88" s="11" t="s">
+      <c r="E88" s="5"/>
+      <c r="F88" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="G88" s="11"/>
-      <c r="H88" s="11"/>
-      <c r="I88" s="11"/>
-      <c r="J88" s="12" t="s">
+      <c r="G88" s="5"/>
+      <c r="H88" s="5"/>
+      <c r="I88" s="5"/>
+      <c r="J88" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="K88" s="13"/>
+      <c r="K88" s="7"/>
     </row>
     <row r="89" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B89" s="10" t="s">
+      <c r="B89" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C89" s="11"/>
-      <c r="D89" s="11" t="s">
+      <c r="C89" s="5"/>
+      <c r="D89" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E89" s="11"/>
-      <c r="F89" s="11" t="s">
+      <c r="E89" s="5"/>
+      <c r="F89" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="G89" s="11"/>
-      <c r="H89" s="11"/>
-      <c r="I89" s="11"/>
-      <c r="J89" s="12" t="s">
+      <c r="G89" s="5"/>
+      <c r="H89" s="5"/>
+      <c r="I89" s="5"/>
+      <c r="J89" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="K89" s="13"/>
+      <c r="K89" s="7"/>
     </row>
     <row r="90" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B90" s="10" t="s">
+      <c r="B90" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C90" s="11"/>
-      <c r="D90" s="11" t="s">
+      <c r="C90" s="5"/>
+      <c r="D90" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="E90" s="11"/>
-      <c r="F90" s="11" t="s">
+      <c r="E90" s="5"/>
+      <c r="F90" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="G90" s="11"/>
-      <c r="H90" s="11"/>
-      <c r="I90" s="11"/>
-      <c r="J90" s="12" t="s">
+      <c r="G90" s="5"/>
+      <c r="H90" s="5"/>
+      <c r="I90" s="5"/>
+      <c r="J90" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="K90" s="13"/>
+      <c r="K90" s="7"/>
     </row>
     <row r="91" spans="2:11" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="B91" s="4" t="s">
+      <c r="B91" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C91" s="5"/>
-      <c r="D91" s="5"/>
-      <c r="E91" s="5"/>
-      <c r="F91" s="5"/>
-      <c r="G91" s="5"/>
-      <c r="H91" s="5"/>
-      <c r="I91" s="5"/>
-      <c r="J91" s="5"/>
-      <c r="K91" s="6"/>
+      <c r="C91" s="9"/>
+      <c r="D91" s="9"/>
+      <c r="E91" s="9"/>
+      <c r="F91" s="9"/>
+      <c r="G91" s="9"/>
+      <c r="H91" s="9"/>
+      <c r="I91" s="9"/>
+      <c r="J91" s="9"/>
+      <c r="K91" s="10"/>
     </row>
     <row r="92" spans="2:11" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B92" s="7" t="s">
+      <c r="B92" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="C92" s="8"/>
-      <c r="D92" s="8"/>
-      <c r="E92" s="8"/>
-      <c r="F92" s="8"/>
-      <c r="G92" s="8"/>
-      <c r="H92" s="8"/>
-      <c r="I92" s="8"/>
-      <c r="J92" s="8"/>
-      <c r="K92" s="9"/>
+      <c r="C92" s="12"/>
+      <c r="D92" s="12"/>
+      <c r="E92" s="12"/>
+      <c r="F92" s="12"/>
+      <c r="G92" s="12"/>
+      <c r="H92" s="12"/>
+      <c r="I92" s="12"/>
+      <c r="J92" s="12"/>
+      <c r="K92" s="13"/>
     </row>
     <row r="93" spans="2:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="94" spans="2:11" ht="41.25" x14ac:dyDescent="0.3">
-      <c r="B94" s="35" t="s">
+      <c r="B94" s="49" t="s">
         <v>46</v>
       </c>
-      <c r="C94" s="36"/>
-      <c r="D94" s="36"/>
-      <c r="E94" s="36"/>
-      <c r="F94" s="36"/>
-      <c r="G94" s="36"/>
-      <c r="H94" s="36"/>
-      <c r="I94" s="36"/>
-      <c r="J94" s="36"/>
-      <c r="K94" s="37"/>
+      <c r="C94" s="50"/>
+      <c r="D94" s="50"/>
+      <c r="E94" s="50"/>
+      <c r="F94" s="50"/>
+      <c r="G94" s="50"/>
+      <c r="H94" s="50"/>
+      <c r="I94" s="50"/>
+      <c r="J94" s="50"/>
+      <c r="K94" s="51"/>
     </row>
     <row r="95" spans="2:11" ht="26.25" x14ac:dyDescent="0.3">
-      <c r="B95" s="38" t="s">
+      <c r="B95" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="C95" s="39"/>
-      <c r="D95" s="39"/>
-      <c r="E95" s="39"/>
-      <c r="F95" s="39"/>
-      <c r="G95" s="39"/>
-      <c r="H95" s="39"/>
-      <c r="I95" s="39"/>
-      <c r="J95" s="39"/>
-      <c r="K95" s="40"/>
+      <c r="C95" s="53"/>
+      <c r="D95" s="53"/>
+      <c r="E95" s="53"/>
+      <c r="F95" s="53"/>
+      <c r="G95" s="53"/>
+      <c r="H95" s="53"/>
+      <c r="I95" s="53"/>
+      <c r="J95" s="53"/>
+      <c r="K95" s="54"/>
     </row>
     <row r="96" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B96" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="C96" s="41"/>
-      <c r="D96" s="41"/>
-      <c r="E96" s="41"/>
-      <c r="F96" s="41"/>
-      <c r="G96" s="41"/>
-      <c r="H96" s="41"/>
-      <c r="I96" s="41"/>
-      <c r="J96" s="41"/>
-      <c r="K96" s="42"/>
+      <c r="C96" s="55"/>
+      <c r="D96" s="55"/>
+      <c r="E96" s="55"/>
+      <c r="F96" s="55"/>
+      <c r="G96" s="55"/>
+      <c r="H96" s="55"/>
+      <c r="I96" s="55"/>
+      <c r="J96" s="55"/>
+      <c r="K96" s="56"/>
     </row>
     <row r="97" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B97" s="19"/>
-      <c r="C97" s="41"/>
-      <c r="D97" s="41"/>
-      <c r="E97" s="41"/>
-      <c r="F97" s="41"/>
-      <c r="G97" s="41"/>
-      <c r="H97" s="41"/>
-      <c r="I97" s="41"/>
-      <c r="J97" s="41"/>
-      <c r="K97" s="42"/>
+      <c r="C97" s="55"/>
+      <c r="D97" s="55"/>
+      <c r="E97" s="55"/>
+      <c r="F97" s="55"/>
+      <c r="G97" s="55"/>
+      <c r="H97" s="55"/>
+      <c r="I97" s="55"/>
+      <c r="J97" s="55"/>
+      <c r="K97" s="56"/>
     </row>
     <row r="98" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B98" s="19"/>
-      <c r="C98" s="41"/>
-      <c r="D98" s="41"/>
-      <c r="E98" s="41"/>
-      <c r="F98" s="41"/>
-      <c r="G98" s="41"/>
-      <c r="H98" s="41"/>
-      <c r="I98" s="41"/>
-      <c r="J98" s="41"/>
-      <c r="K98" s="42"/>
+      <c r="C98" s="55"/>
+      <c r="D98" s="55"/>
+      <c r="E98" s="55"/>
+      <c r="F98" s="55"/>
+      <c r="G98" s="55"/>
+      <c r="H98" s="55"/>
+      <c r="I98" s="55"/>
+      <c r="J98" s="55"/>
+      <c r="K98" s="56"/>
     </row>
     <row r="99" spans="2:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B99" s="43"/>
-      <c r="C99" s="44"/>
-      <c r="D99" s="44"/>
-      <c r="E99" s="44"/>
-      <c r="F99" s="44"/>
-      <c r="G99" s="44"/>
-      <c r="H99" s="44"/>
-      <c r="I99" s="44"/>
-      <c r="J99" s="44"/>
-      <c r="K99" s="45"/>
+      <c r="B99" s="57"/>
+      <c r="C99" s="58"/>
+      <c r="D99" s="58"/>
+      <c r="E99" s="58"/>
+      <c r="F99" s="58"/>
+      <c r="G99" s="58"/>
+      <c r="H99" s="58"/>
+      <c r="I99" s="58"/>
+      <c r="J99" s="58"/>
+      <c r="K99" s="59"/>
     </row>
     <row r="100" spans="2:11" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B100" s="26" t="s">
         <v>4</v>
       </c>
       <c r="C100" s="27"/>
-      <c r="D100" s="46" t="s">
+      <c r="D100" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="E100" s="46"/>
-      <c r="F100" s="47"/>
-      <c r="G100" s="48" t="s">
+      <c r="E100" s="36"/>
+      <c r="F100" s="37"/>
+      <c r="G100" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="H100" s="49"/>
-      <c r="I100" s="50" t="s">
+      <c r="H100" s="39"/>
+      <c r="I100" s="40" t="s">
         <v>48</v>
       </c>
-      <c r="J100" s="50"/>
-      <c r="K100" s="51"/>
+      <c r="J100" s="40"/>
+      <c r="K100" s="41"/>
     </row>
     <row r="101" spans="2:11" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B101" s="26" t="s">
@@ -2971,36 +3008,36 @@
       <c r="B102" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="C102" s="33"/>
-      <c r="D102" s="33"/>
-      <c r="E102" s="33"/>
-      <c r="F102" s="33"/>
-      <c r="G102" s="33"/>
-      <c r="H102" s="33"/>
-      <c r="I102" s="33"/>
-      <c r="J102" s="33"/>
-      <c r="K102" s="34"/>
+      <c r="C102" s="42"/>
+      <c r="D102" s="42"/>
+      <c r="E102" s="42"/>
+      <c r="F102" s="42"/>
+      <c r="G102" s="42"/>
+      <c r="H102" s="42"/>
+      <c r="I102" s="42"/>
+      <c r="J102" s="42"/>
+      <c r="K102" s="43"/>
     </row>
     <row r="103" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B103" s="73" t="s">
+      <c r="B103" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="C103" s="72"/>
-      <c r="D103" s="69" t="s">
+      <c r="C103" s="45"/>
+      <c r="D103" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="E103" s="71"/>
-      <c r="F103" s="71"/>
-      <c r="G103" s="71"/>
-      <c r="H103" s="71"/>
-      <c r="I103" s="72"/>
-      <c r="J103" s="69" t="s">
+      <c r="E103" s="47"/>
+      <c r="F103" s="47"/>
+      <c r="G103" s="47"/>
+      <c r="H103" s="47"/>
+      <c r="I103" s="45"/>
+      <c r="J103" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="K103" s="70"/>
+      <c r="K103" s="48"/>
     </row>
     <row r="104" spans="2:11" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="B104" s="4" t="s">
+      <c r="B104" s="8" t="s">
         <v>11</v>
       </c>
       <c r="C104" s="17"/>
@@ -3034,27 +3071,27 @@
       <c r="K105" s="16"/>
     </row>
     <row r="106" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B106" s="74" t="s">
+      <c r="B106" s="32" t="s">
         <v>49</v>
       </c>
-      <c r="C106" s="75"/>
-      <c r="D106" s="75" t="s">
+      <c r="C106" s="33"/>
+      <c r="D106" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="E106" s="75"/>
-      <c r="F106" s="75" t="s">
+      <c r="E106" s="33"/>
+      <c r="F106" s="33" t="s">
         <v>51</v>
       </c>
-      <c r="G106" s="75"/>
-      <c r="H106" s="75"/>
-      <c r="I106" s="75"/>
-      <c r="J106" s="75" t="s">
+      <c r="G106" s="33"/>
+      <c r="H106" s="33"/>
+      <c r="I106" s="33"/>
+      <c r="J106" s="33" t="s">
         <v>50</v>
       </c>
-      <c r="K106" s="76"/>
+      <c r="K106" s="35"/>
     </row>
     <row r="107" spans="2:11" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="B107" s="4" t="s">
+      <c r="B107" s="8" t="s">
         <v>10</v>
       </c>
       <c r="C107" s="17"/>
@@ -3164,36 +3201,36 @@
       <c r="K114" s="16"/>
     </row>
     <row r="115" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B115" s="10" t="s">
+      <c r="B115" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C115" s="11"/>
-      <c r="D115" s="11" t="s">
+      <c r="C115" s="5"/>
+      <c r="D115" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="E115" s="11"/>
-      <c r="F115" s="11"/>
-      <c r="G115" s="11"/>
-      <c r="H115" s="11"/>
-      <c r="I115" s="11"/>
-      <c r="J115" s="12" t="s">
+      <c r="E115" s="5"/>
+      <c r="F115" s="5"/>
+      <c r="G115" s="5"/>
+      <c r="H115" s="5"/>
+      <c r="I115" s="5"/>
+      <c r="J115" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="K115" s="13"/>
+      <c r="K115" s="7"/>
     </row>
     <row r="116" spans="2:11" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="B116" s="4" t="s">
+      <c r="B116" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C116" s="5"/>
-      <c r="D116" s="5"/>
-      <c r="E116" s="5"/>
-      <c r="F116" s="5"/>
-      <c r="G116" s="5"/>
-      <c r="H116" s="5"/>
-      <c r="I116" s="5"/>
-      <c r="J116" s="5"/>
-      <c r="K116" s="6"/>
+      <c r="C116" s="9"/>
+      <c r="D116" s="9"/>
+      <c r="E116" s="9"/>
+      <c r="F116" s="9"/>
+      <c r="G116" s="9"/>
+      <c r="H116" s="9"/>
+      <c r="I116" s="9"/>
+      <c r="J116" s="9"/>
+      <c r="K116" s="10"/>
     </row>
     <row r="117" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B117" s="14" t="s">
@@ -3216,171 +3253,171 @@
       <c r="K117" s="16"/>
     </row>
     <row r="118" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B118" s="10" t="s">
+      <c r="B118" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C118" s="11"/>
-      <c r="D118" s="11" t="s">
+      <c r="C118" s="5"/>
+      <c r="D118" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E118" s="11"/>
-      <c r="F118" s="11" t="s">
+      <c r="E118" s="5"/>
+      <c r="F118" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="G118" s="11"/>
-      <c r="H118" s="11"/>
-      <c r="I118" s="11"/>
-      <c r="J118" s="12" t="s">
+      <c r="G118" s="5"/>
+      <c r="H118" s="5"/>
+      <c r="I118" s="5"/>
+      <c r="J118" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="K118" s="13"/>
+      <c r="K118" s="7"/>
     </row>
     <row r="119" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B119" s="10" t="s">
+      <c r="B119" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C119" s="11"/>
-      <c r="D119" s="11" t="s">
+      <c r="C119" s="5"/>
+      <c r="D119" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E119" s="11"/>
-      <c r="F119" s="11" t="s">
+      <c r="E119" s="5"/>
+      <c r="F119" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="G119" s="11"/>
-      <c r="H119" s="11"/>
-      <c r="I119" s="11"/>
-      <c r="J119" s="12" t="s">
+      <c r="G119" s="5"/>
+      <c r="H119" s="5"/>
+      <c r="I119" s="5"/>
+      <c r="J119" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="K119" s="13"/>
+      <c r="K119" s="7"/>
     </row>
     <row r="120" spans="2:11" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="B120" s="4" t="s">
+      <c r="B120" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C120" s="5"/>
-      <c r="D120" s="5"/>
-      <c r="E120" s="5"/>
-      <c r="F120" s="5"/>
-      <c r="G120" s="5"/>
-      <c r="H120" s="5"/>
-      <c r="I120" s="5"/>
-      <c r="J120" s="5"/>
-      <c r="K120" s="6"/>
+      <c r="C120" s="9"/>
+      <c r="D120" s="9"/>
+      <c r="E120" s="9"/>
+      <c r="F120" s="9"/>
+      <c r="G120" s="9"/>
+      <c r="H120" s="9"/>
+      <c r="I120" s="9"/>
+      <c r="J120" s="9"/>
+      <c r="K120" s="10"/>
     </row>
     <row r="121" spans="2:11" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B121" s="7" t="s">
+      <c r="B121" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="C121" s="8"/>
-      <c r="D121" s="8"/>
-      <c r="E121" s="8"/>
-      <c r="F121" s="8"/>
-      <c r="G121" s="8"/>
-      <c r="H121" s="8"/>
-      <c r="I121" s="8"/>
-      <c r="J121" s="8"/>
-      <c r="K121" s="9"/>
+      <c r="C121" s="12"/>
+      <c r="D121" s="12"/>
+      <c r="E121" s="12"/>
+      <c r="F121" s="12"/>
+      <c r="G121" s="12"/>
+      <c r="H121" s="12"/>
+      <c r="I121" s="12"/>
+      <c r="J121" s="12"/>
+      <c r="K121" s="13"/>
     </row>
     <row r="122" spans="2:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="123" spans="2:11" ht="41.25" x14ac:dyDescent="0.3">
-      <c r="B123" s="35" t="s">
+      <c r="B123" s="49" t="s">
         <v>55</v>
       </c>
-      <c r="C123" s="36"/>
-      <c r="D123" s="36"/>
-      <c r="E123" s="36"/>
-      <c r="F123" s="36"/>
-      <c r="G123" s="36"/>
-      <c r="H123" s="36"/>
-      <c r="I123" s="36"/>
-      <c r="J123" s="36"/>
-      <c r="K123" s="37"/>
+      <c r="C123" s="50"/>
+      <c r="D123" s="50"/>
+      <c r="E123" s="50"/>
+      <c r="F123" s="50"/>
+      <c r="G123" s="50"/>
+      <c r="H123" s="50"/>
+      <c r="I123" s="50"/>
+      <c r="J123" s="50"/>
+      <c r="K123" s="51"/>
     </row>
     <row r="124" spans="2:11" ht="26.25" x14ac:dyDescent="0.3">
-      <c r="B124" s="38" t="s">
+      <c r="B124" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="C124" s="39"/>
-      <c r="D124" s="39"/>
-      <c r="E124" s="39"/>
-      <c r="F124" s="39"/>
-      <c r="G124" s="39"/>
-      <c r="H124" s="39"/>
-      <c r="I124" s="39"/>
-      <c r="J124" s="39"/>
-      <c r="K124" s="40"/>
+      <c r="C124" s="53"/>
+      <c r="D124" s="53"/>
+      <c r="E124" s="53"/>
+      <c r="F124" s="53"/>
+      <c r="G124" s="53"/>
+      <c r="H124" s="53"/>
+      <c r="I124" s="53"/>
+      <c r="J124" s="53"/>
+      <c r="K124" s="54"/>
     </row>
     <row r="125" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B125" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="C125" s="41"/>
-      <c r="D125" s="41"/>
-      <c r="E125" s="41"/>
-      <c r="F125" s="41"/>
-      <c r="G125" s="41"/>
-      <c r="H125" s="41"/>
-      <c r="I125" s="41"/>
-      <c r="J125" s="41"/>
-      <c r="K125" s="42"/>
+      <c r="C125" s="55"/>
+      <c r="D125" s="55"/>
+      <c r="E125" s="55"/>
+      <c r="F125" s="55"/>
+      <c r="G125" s="55"/>
+      <c r="H125" s="55"/>
+      <c r="I125" s="55"/>
+      <c r="J125" s="55"/>
+      <c r="K125" s="56"/>
     </row>
     <row r="126" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B126" s="19"/>
-      <c r="C126" s="41"/>
-      <c r="D126" s="41"/>
-      <c r="E126" s="41"/>
-      <c r="F126" s="41"/>
-      <c r="G126" s="41"/>
-      <c r="H126" s="41"/>
-      <c r="I126" s="41"/>
-      <c r="J126" s="41"/>
-      <c r="K126" s="42"/>
+      <c r="C126" s="55"/>
+      <c r="D126" s="55"/>
+      <c r="E126" s="55"/>
+      <c r="F126" s="55"/>
+      <c r="G126" s="55"/>
+      <c r="H126" s="55"/>
+      <c r="I126" s="55"/>
+      <c r="J126" s="55"/>
+      <c r="K126" s="56"/>
     </row>
     <row r="127" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B127" s="19"/>
-      <c r="C127" s="41"/>
-      <c r="D127" s="41"/>
-      <c r="E127" s="41"/>
-      <c r="F127" s="41"/>
-      <c r="G127" s="41"/>
-      <c r="H127" s="41"/>
-      <c r="I127" s="41"/>
-      <c r="J127" s="41"/>
-      <c r="K127" s="42"/>
+      <c r="C127" s="55"/>
+      <c r="D127" s="55"/>
+      <c r="E127" s="55"/>
+      <c r="F127" s="55"/>
+      <c r="G127" s="55"/>
+      <c r="H127" s="55"/>
+      <c r="I127" s="55"/>
+      <c r="J127" s="55"/>
+      <c r="K127" s="56"/>
     </row>
     <row r="128" spans="2:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B128" s="43"/>
-      <c r="C128" s="44"/>
-      <c r="D128" s="44"/>
-      <c r="E128" s="44"/>
-      <c r="F128" s="44"/>
-      <c r="G128" s="44"/>
-      <c r="H128" s="44"/>
-      <c r="I128" s="44"/>
-      <c r="J128" s="44"/>
-      <c r="K128" s="45"/>
+      <c r="B128" s="57"/>
+      <c r="C128" s="58"/>
+      <c r="D128" s="58"/>
+      <c r="E128" s="58"/>
+      <c r="F128" s="58"/>
+      <c r="G128" s="58"/>
+      <c r="H128" s="58"/>
+      <c r="I128" s="58"/>
+      <c r="J128" s="58"/>
+      <c r="K128" s="59"/>
     </row>
     <row r="129" spans="2:11" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B129" s="26" t="s">
         <v>4</v>
       </c>
       <c r="C129" s="27"/>
-      <c r="D129" s="46" t="s">
+      <c r="D129" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="E129" s="46"/>
-      <c r="F129" s="47"/>
-      <c r="G129" s="48" t="s">
+      <c r="E129" s="36"/>
+      <c r="F129" s="37"/>
+      <c r="G129" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="H129" s="49"/>
-      <c r="I129" s="50" t="s">
-        <v>59</v>
-      </c>
-      <c r="J129" s="50"/>
-      <c r="K129" s="51"/>
+      <c r="H129" s="39"/>
+      <c r="I129" s="40" t="s">
+        <v>58</v>
+      </c>
+      <c r="J129" s="40"/>
+      <c r="K129" s="41"/>
     </row>
     <row r="130" spans="2:11" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B130" s="26" t="s">
@@ -3400,36 +3437,36 @@
       <c r="B131" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="C131" s="33"/>
-      <c r="D131" s="33"/>
-      <c r="E131" s="33"/>
-      <c r="F131" s="33"/>
-      <c r="G131" s="33"/>
-      <c r="H131" s="33"/>
-      <c r="I131" s="33"/>
-      <c r="J131" s="33"/>
-      <c r="K131" s="34"/>
+      <c r="C131" s="42"/>
+      <c r="D131" s="42"/>
+      <c r="E131" s="42"/>
+      <c r="F131" s="42"/>
+      <c r="G131" s="42"/>
+      <c r="H131" s="42"/>
+      <c r="I131" s="42"/>
+      <c r="J131" s="42"/>
+      <c r="K131" s="43"/>
     </row>
     <row r="132" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B132" s="73" t="s">
+      <c r="B132" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="C132" s="72"/>
-      <c r="D132" s="69" t="s">
+      <c r="C132" s="45"/>
+      <c r="D132" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="E132" s="71"/>
-      <c r="F132" s="71"/>
-      <c r="G132" s="71"/>
-      <c r="H132" s="71"/>
-      <c r="I132" s="72"/>
-      <c r="J132" s="69" t="s">
+      <c r="E132" s="47"/>
+      <c r="F132" s="47"/>
+      <c r="G132" s="47"/>
+      <c r="H132" s="47"/>
+      <c r="I132" s="45"/>
+      <c r="J132" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="K132" s="70"/>
+      <c r="K132" s="48"/>
     </row>
     <row r="133" spans="2:11" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="B133" s="4" t="s">
+      <c r="B133" s="8" t="s">
         <v>11</v>
       </c>
       <c r="C133" s="17"/>
@@ -3463,27 +3500,27 @@
       <c r="K134" s="16"/>
     </row>
     <row r="135" spans="2:11" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B135" s="74" t="s">
+      <c r="B135" s="32" t="s">
         <v>57</v>
       </c>
-      <c r="C135" s="75"/>
-      <c r="D135" s="75" t="s">
+      <c r="C135" s="33"/>
+      <c r="D135" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="E135" s="75"/>
-      <c r="F135" s="77" t="s">
-        <v>60</v>
-      </c>
-      <c r="G135" s="75"/>
-      <c r="H135" s="75"/>
-      <c r="I135" s="75"/>
-      <c r="J135" s="75" t="s">
+      <c r="E135" s="33"/>
+      <c r="F135" s="34" t="s">
+        <v>59</v>
+      </c>
+      <c r="G135" s="33"/>
+      <c r="H135" s="33"/>
+      <c r="I135" s="33"/>
+      <c r="J135" s="33" t="s">
         <v>50</v>
       </c>
-      <c r="K135" s="76"/>
+      <c r="K135" s="35"/>
     </row>
     <row r="136" spans="2:11" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="B136" s="4" t="s">
+      <c r="B136" s="8" t="s">
         <v>10</v>
       </c>
       <c r="C136" s="17"/>
@@ -3498,7 +3535,7 @@
     </row>
     <row r="137" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B137" s="19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C137" s="20"/>
       <c r="D137" s="20"/>
@@ -3593,36 +3630,36 @@
       <c r="K143" s="16"/>
     </row>
     <row r="144" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B144" s="10" t="s">
+      <c r="B144" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C144" s="11"/>
-      <c r="D144" s="11" t="s">
+      <c r="C144" s="5"/>
+      <c r="D144" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="E144" s="11"/>
-      <c r="F144" s="11"/>
-      <c r="G144" s="11"/>
-      <c r="H144" s="11"/>
-      <c r="I144" s="11"/>
-      <c r="J144" s="12" t="s">
+      <c r="E144" s="5"/>
+      <c r="F144" s="5"/>
+      <c r="G144" s="5"/>
+      <c r="H144" s="5"/>
+      <c r="I144" s="5"/>
+      <c r="J144" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="K144" s="13"/>
+      <c r="K144" s="7"/>
     </row>
     <row r="145" spans="2:11" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="B145" s="4" t="s">
+      <c r="B145" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C145" s="5"/>
-      <c r="D145" s="5"/>
-      <c r="E145" s="5"/>
-      <c r="F145" s="5"/>
-      <c r="G145" s="5"/>
-      <c r="H145" s="5"/>
-      <c r="I145" s="5"/>
-      <c r="J145" s="5"/>
-      <c r="K145" s="6"/>
+      <c r="C145" s="9"/>
+      <c r="D145" s="9"/>
+      <c r="E145" s="9"/>
+      <c r="F145" s="9"/>
+      <c r="G145" s="9"/>
+      <c r="H145" s="9"/>
+      <c r="I145" s="9"/>
+      <c r="J145" s="9"/>
+      <c r="K145" s="10"/>
     </row>
     <row r="146" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B146" s="14" t="s">
@@ -3645,118 +3682,715 @@
       <c r="K146" s="16"/>
     </row>
     <row r="147" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B147" s="10" t="s">
+      <c r="B147" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C147" s="11"/>
-      <c r="D147" s="11" t="s">
+      <c r="C147" s="5"/>
+      <c r="D147" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E147" s="11"/>
-      <c r="F147" s="11" t="s">
+      <c r="E147" s="5"/>
+      <c r="F147" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="G147" s="11"/>
-      <c r="H147" s="11"/>
-      <c r="I147" s="11"/>
-      <c r="J147" s="12" t="s">
+      <c r="G147" s="5"/>
+      <c r="H147" s="5"/>
+      <c r="I147" s="5"/>
+      <c r="J147" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="K147" s="13"/>
+      <c r="K147" s="7"/>
     </row>
     <row r="148" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B148" s="10" t="s">
+      <c r="B148" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C148" s="11"/>
-      <c r="D148" s="11" t="s">
+      <c r="C148" s="5"/>
+      <c r="D148" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E148" s="11"/>
-      <c r="F148" s="11" t="s">
+      <c r="E148" s="5"/>
+      <c r="F148" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="G148" s="11"/>
-      <c r="H148" s="11"/>
-      <c r="I148" s="11"/>
-      <c r="J148" s="12" t="s">
+      <c r="G148" s="5"/>
+      <c r="H148" s="5"/>
+      <c r="I148" s="5"/>
+      <c r="J148" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="K148" s="13"/>
+      <c r="K148" s="7"/>
     </row>
     <row r="149" spans="2:11" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="B149" s="4" t="s">
+      <c r="B149" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C149" s="5"/>
-      <c r="D149" s="5"/>
-      <c r="E149" s="5"/>
-      <c r="F149" s="5"/>
-      <c r="G149" s="5"/>
-      <c r="H149" s="5"/>
-      <c r="I149" s="5"/>
-      <c r="J149" s="5"/>
-      <c r="K149" s="6"/>
-    </row>
-    <row r="150" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B150" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="C150" s="8"/>
-      <c r="D150" s="8"/>
-      <c r="E150" s="8"/>
-      <c r="F150" s="8"/>
-      <c r="G150" s="8"/>
-      <c r="H150" s="8"/>
-      <c r="I150" s="8"/>
-      <c r="J150" s="8"/>
-      <c r="K150" s="9"/>
+      <c r="C149" s="9"/>
+      <c r="D149" s="9"/>
+      <c r="E149" s="9"/>
+      <c r="F149" s="9"/>
+      <c r="G149" s="9"/>
+      <c r="H149" s="9"/>
+      <c r="I149" s="9"/>
+      <c r="J149" s="9"/>
+      <c r="K149" s="10"/>
+    </row>
+    <row r="150" spans="2:11" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B150" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="C150" s="12"/>
+      <c r="D150" s="12"/>
+      <c r="E150" s="12"/>
+      <c r="F150" s="12"/>
+      <c r="G150" s="12"/>
+      <c r="H150" s="12"/>
+      <c r="I150" s="12"/>
+      <c r="J150" s="12"/>
+      <c r="K150" s="13"/>
+    </row>
+    <row r="151" spans="2:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="152" spans="2:11" ht="41.25" x14ac:dyDescent="0.3">
+      <c r="B152" s="49" t="s">
+        <v>62</v>
+      </c>
+      <c r="C152" s="50"/>
+      <c r="D152" s="50"/>
+      <c r="E152" s="50"/>
+      <c r="F152" s="50"/>
+      <c r="G152" s="50"/>
+      <c r="H152" s="50"/>
+      <c r="I152" s="50"/>
+      <c r="J152" s="50"/>
+      <c r="K152" s="51"/>
+    </row>
+    <row r="153" spans="2:11" ht="26.25" x14ac:dyDescent="0.3">
+      <c r="B153" s="52" t="s">
+        <v>0</v>
+      </c>
+      <c r="C153" s="53"/>
+      <c r="D153" s="53"/>
+      <c r="E153" s="53"/>
+      <c r="F153" s="53"/>
+      <c r="G153" s="53"/>
+      <c r="H153" s="53"/>
+      <c r="I153" s="53"/>
+      <c r="J153" s="53"/>
+      <c r="K153" s="54"/>
+    </row>
+    <row r="154" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B154" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="C154" s="55"/>
+      <c r="D154" s="55"/>
+      <c r="E154" s="55"/>
+      <c r="F154" s="55"/>
+      <c r="G154" s="55"/>
+      <c r="H154" s="55"/>
+      <c r="I154" s="55"/>
+      <c r="J154" s="55"/>
+      <c r="K154" s="56"/>
+    </row>
+    <row r="155" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B155" s="19"/>
+      <c r="C155" s="55"/>
+      <c r="D155" s="55"/>
+      <c r="E155" s="55"/>
+      <c r="F155" s="55"/>
+      <c r="G155" s="55"/>
+      <c r="H155" s="55"/>
+      <c r="I155" s="55"/>
+      <c r="J155" s="55"/>
+      <c r="K155" s="56"/>
+    </row>
+    <row r="156" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B156" s="19"/>
+      <c r="C156" s="55"/>
+      <c r="D156" s="55"/>
+      <c r="E156" s="55"/>
+      <c r="F156" s="55"/>
+      <c r="G156" s="55"/>
+      <c r="H156" s="55"/>
+      <c r="I156" s="55"/>
+      <c r="J156" s="55"/>
+      <c r="K156" s="56"/>
+    </row>
+    <row r="157" spans="2:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B157" s="57"/>
+      <c r="C157" s="58"/>
+      <c r="D157" s="58"/>
+      <c r="E157" s="58"/>
+      <c r="F157" s="58"/>
+      <c r="G157" s="58"/>
+      <c r="H157" s="58"/>
+      <c r="I157" s="58"/>
+      <c r="J157" s="58"/>
+      <c r="K157" s="59"/>
+    </row>
+    <row r="158" spans="2:11" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B158" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="C158" s="27"/>
+      <c r="D158" s="36" t="s">
+        <v>19</v>
+      </c>
+      <c r="E158" s="36"/>
+      <c r="F158" s="37"/>
+      <c r="G158" s="38" t="s">
+        <v>5</v>
+      </c>
+      <c r="H158" s="39"/>
+      <c r="I158" s="40" t="s">
+        <v>64</v>
+      </c>
+      <c r="J158" s="40"/>
+      <c r="K158" s="41"/>
+    </row>
+    <row r="159" spans="2:11" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B159" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="C159" s="27"/>
+      <c r="D159" s="27"/>
+      <c r="E159" s="27"/>
+      <c r="F159" s="27"/>
+      <c r="G159" s="27"/>
+      <c r="H159" s="27"/>
+      <c r="I159" s="27"/>
+      <c r="J159" s="27"/>
+      <c r="K159" s="28"/>
+    </row>
+    <row r="160" spans="2:11" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="B160" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="C160" s="42"/>
+      <c r="D160" s="42"/>
+      <c r="E160" s="42"/>
+      <c r="F160" s="42"/>
+      <c r="G160" s="42"/>
+      <c r="H160" s="42"/>
+      <c r="I160" s="42"/>
+      <c r="J160" s="42"/>
+      <c r="K160" s="43"/>
+    </row>
+    <row r="161" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B161" s="44" t="s">
+        <v>6</v>
+      </c>
+      <c r="C161" s="45"/>
+      <c r="D161" s="46" t="s">
+        <v>8</v>
+      </c>
+      <c r="E161" s="47"/>
+      <c r="F161" s="47"/>
+      <c r="G161" s="47"/>
+      <c r="H161" s="47"/>
+      <c r="I161" s="45"/>
+      <c r="J161" s="46" t="s">
+        <v>9</v>
+      </c>
+      <c r="K161" s="48"/>
+    </row>
+    <row r="162" spans="2:11" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="B162" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C162" s="17"/>
+      <c r="D162" s="17"/>
+      <c r="E162" s="17"/>
+      <c r="F162" s="17"/>
+      <c r="G162" s="17"/>
+      <c r="H162" s="17"/>
+      <c r="I162" s="17"/>
+      <c r="J162" s="17"/>
+      <c r="K162" s="18"/>
+    </row>
+    <row r="163" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B163" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C163" s="15"/>
+      <c r="D163" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="E163" s="15"/>
+      <c r="F163" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="G163" s="15"/>
+      <c r="H163" s="15"/>
+      <c r="I163" s="15"/>
+      <c r="J163" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="K163" s="16"/>
+    </row>
+    <row r="164" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B164" s="32" t="s">
+        <v>57</v>
+      </c>
+      <c r="C164" s="33"/>
+      <c r="D164" s="33" t="s">
+        <v>23</v>
+      </c>
+      <c r="E164" s="33"/>
+      <c r="F164" s="34" t="s">
+        <v>65</v>
+      </c>
+      <c r="G164" s="33"/>
+      <c r="H164" s="33"/>
+      <c r="I164" s="33"/>
+      <c r="J164" s="33" t="s">
+        <v>25</v>
+      </c>
+      <c r="K164" s="35"/>
+    </row>
+    <row r="165" spans="2:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B165" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="C165" s="33"/>
+      <c r="D165" s="33" t="s">
+        <v>23</v>
+      </c>
+      <c r="E165" s="33"/>
+      <c r="F165" s="34" t="s">
+        <v>67</v>
+      </c>
+      <c r="G165" s="33"/>
+      <c r="H165" s="33"/>
+      <c r="I165" s="33"/>
+      <c r="J165" s="33" t="s">
+        <v>25</v>
+      </c>
+      <c r="K165" s="35"/>
+    </row>
+    <row r="166" spans="2:11" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="B166" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C166" s="17"/>
+      <c r="D166" s="17"/>
+      <c r="E166" s="17"/>
+      <c r="F166" s="17"/>
+      <c r="G166" s="17"/>
+      <c r="H166" s="17"/>
+      <c r="I166" s="17"/>
+      <c r="J166" s="17"/>
+      <c r="K166" s="18"/>
+    </row>
+    <row r="167" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B167" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="C167" s="20"/>
+      <c r="D167" s="20"/>
+      <c r="E167" s="20"/>
+      <c r="F167" s="20"/>
+      <c r="G167" s="20"/>
+      <c r="H167" s="20"/>
+      <c r="I167" s="20"/>
+      <c r="J167" s="20"/>
+      <c r="K167" s="21"/>
+    </row>
+    <row r="168" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B168" s="22"/>
+      <c r="C168" s="20"/>
+      <c r="D168" s="20"/>
+      <c r="E168" s="20"/>
+      <c r="F168" s="20"/>
+      <c r="G168" s="20"/>
+      <c r="H168" s="20"/>
+      <c r="I168" s="20"/>
+      <c r="J168" s="20"/>
+      <c r="K168" s="21"/>
+    </row>
+    <row r="169" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B169" s="22"/>
+      <c r="C169" s="20"/>
+      <c r="D169" s="20"/>
+      <c r="E169" s="20"/>
+      <c r="F169" s="20"/>
+      <c r="G169" s="20"/>
+      <c r="H169" s="20"/>
+      <c r="I169" s="20"/>
+      <c r="J169" s="20"/>
+      <c r="K169" s="21"/>
+    </row>
+    <row r="170" spans="2:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B170" s="23"/>
+      <c r="C170" s="24"/>
+      <c r="D170" s="24"/>
+      <c r="E170" s="24"/>
+      <c r="F170" s="24"/>
+      <c r="G170" s="24"/>
+      <c r="H170" s="24"/>
+      <c r="I170" s="24"/>
+      <c r="J170" s="24"/>
+      <c r="K170" s="25"/>
+    </row>
+    <row r="171" spans="2:11" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B171" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="C171" s="27"/>
+      <c r="D171" s="27"/>
+      <c r="E171" s="27"/>
+      <c r="F171" s="27"/>
+      <c r="G171" s="27"/>
+      <c r="H171" s="27"/>
+      <c r="I171" s="27"/>
+      <c r="J171" s="27"/>
+      <c r="K171" s="28"/>
+    </row>
+    <row r="172" spans="2:11" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="B172" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="C172" s="30"/>
+      <c r="D172" s="30"/>
+      <c r="E172" s="30"/>
+      <c r="F172" s="30"/>
+      <c r="G172" s="30"/>
+      <c r="H172" s="30"/>
+      <c r="I172" s="30"/>
+      <c r="J172" s="30"/>
+      <c r="K172" s="31"/>
+    </row>
+    <row r="173" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B173" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C173" s="15"/>
+      <c r="D173" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="E173" s="15"/>
+      <c r="F173" s="15"/>
+      <c r="G173" s="15"/>
+      <c r="H173" s="15"/>
+      <c r="I173" s="15"/>
+      <c r="J173" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="K173" s="16"/>
+    </row>
+    <row r="174" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B174" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C174" s="5"/>
+      <c r="D174" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E174" s="5"/>
+      <c r="F174" s="5"/>
+      <c r="G174" s="5"/>
+      <c r="H174" s="5"/>
+      <c r="I174" s="5"/>
+      <c r="J174" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="K174" s="7"/>
+    </row>
+    <row r="175" spans="2:11" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="B175" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C175" s="9"/>
+      <c r="D175" s="9"/>
+      <c r="E175" s="9"/>
+      <c r="F175" s="9"/>
+      <c r="G175" s="9"/>
+      <c r="H175" s="9"/>
+      <c r="I175" s="9"/>
+      <c r="J175" s="9"/>
+      <c r="K175" s="10"/>
+    </row>
+    <row r="176" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B176" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C176" s="15"/>
+      <c r="D176" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="E176" s="15"/>
+      <c r="F176" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="G176" s="15"/>
+      <c r="H176" s="15"/>
+      <c r="I176" s="15"/>
+      <c r="J176" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="K176" s="16"/>
+    </row>
+    <row r="177" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B177" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C177" s="5"/>
+      <c r="D177" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E177" s="5"/>
+      <c r="F177" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G177" s="5"/>
+      <c r="H177" s="5"/>
+      <c r="I177" s="5"/>
+      <c r="J177" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="K177" s="7"/>
+    </row>
+    <row r="178" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B178" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C178" s="5"/>
+      <c r="D178" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E178" s="5"/>
+      <c r="F178" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G178" s="5"/>
+      <c r="H178" s="5"/>
+      <c r="I178" s="5"/>
+      <c r="J178" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="K178" s="7"/>
+    </row>
+    <row r="179" spans="2:11" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="B179" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C179" s="9"/>
+      <c r="D179" s="9"/>
+      <c r="E179" s="9"/>
+      <c r="F179" s="9"/>
+      <c r="G179" s="9"/>
+      <c r="H179" s="9"/>
+      <c r="I179" s="9"/>
+      <c r="J179" s="9"/>
+      <c r="K179" s="10"/>
+    </row>
+    <row r="180" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B180" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="C180" s="12"/>
+      <c r="D180" s="12"/>
+      <c r="E180" s="12"/>
+      <c r="F180" s="12"/>
+      <c r="G180" s="12"/>
+      <c r="H180" s="12"/>
+      <c r="I180" s="12"/>
+      <c r="J180" s="12"/>
+      <c r="K180" s="13"/>
     </row>
   </sheetData>
-  <mergeCells count="208">
-    <mergeCell ref="B148:C148"/>
-    <mergeCell ref="D148:E148"/>
-    <mergeCell ref="F148:I148"/>
-    <mergeCell ref="J148:K148"/>
-    <mergeCell ref="B149:K149"/>
-    <mergeCell ref="B150:K150"/>
-    <mergeCell ref="B145:K145"/>
-    <mergeCell ref="B146:C146"/>
-    <mergeCell ref="D146:E146"/>
-    <mergeCell ref="F146:I146"/>
-    <mergeCell ref="J146:K146"/>
-    <mergeCell ref="B147:C147"/>
-    <mergeCell ref="D147:E147"/>
-    <mergeCell ref="F147:I147"/>
-    <mergeCell ref="J147:K147"/>
-    <mergeCell ref="B136:K136"/>
-    <mergeCell ref="B137:K140"/>
-    <mergeCell ref="B141:K141"/>
-    <mergeCell ref="B142:K142"/>
-    <mergeCell ref="B143:C143"/>
-    <mergeCell ref="D143:I143"/>
-    <mergeCell ref="J143:K143"/>
-    <mergeCell ref="B144:C144"/>
-    <mergeCell ref="D144:I144"/>
-    <mergeCell ref="J144:K144"/>
-    <mergeCell ref="B133:K133"/>
-    <mergeCell ref="B134:C134"/>
-    <mergeCell ref="D134:E134"/>
-    <mergeCell ref="F134:I134"/>
-    <mergeCell ref="J134:K134"/>
-    <mergeCell ref="B135:C135"/>
-    <mergeCell ref="D135:E135"/>
-    <mergeCell ref="F135:I135"/>
-    <mergeCell ref="J135:K135"/>
-    <mergeCell ref="B129:C129"/>
-    <mergeCell ref="D129:F129"/>
-    <mergeCell ref="G129:H129"/>
-    <mergeCell ref="I129:K129"/>
-    <mergeCell ref="B130:K130"/>
-    <mergeCell ref="B131:K131"/>
-    <mergeCell ref="B132:C132"/>
-    <mergeCell ref="D132:I132"/>
-    <mergeCell ref="J132:K132"/>
+  <mergeCells count="258">
+    <mergeCell ref="B178:C178"/>
+    <mergeCell ref="D178:E178"/>
+    <mergeCell ref="F178:I178"/>
+    <mergeCell ref="J178:K178"/>
+    <mergeCell ref="B179:K179"/>
+    <mergeCell ref="B180:K180"/>
+    <mergeCell ref="B165:C165"/>
+    <mergeCell ref="D165:E165"/>
+    <mergeCell ref="F165:I165"/>
+    <mergeCell ref="J165:K165"/>
+    <mergeCell ref="B175:K175"/>
+    <mergeCell ref="B176:C176"/>
+    <mergeCell ref="D176:E176"/>
+    <mergeCell ref="F176:I176"/>
+    <mergeCell ref="J176:K176"/>
+    <mergeCell ref="B177:C177"/>
+    <mergeCell ref="D177:E177"/>
+    <mergeCell ref="F177:I177"/>
+    <mergeCell ref="J177:K177"/>
+    <mergeCell ref="B166:K166"/>
+    <mergeCell ref="B167:K170"/>
+    <mergeCell ref="B171:K171"/>
+    <mergeCell ref="B172:K172"/>
+    <mergeCell ref="B173:C173"/>
+    <mergeCell ref="D173:I173"/>
+    <mergeCell ref="J173:K173"/>
+    <mergeCell ref="B174:C174"/>
+    <mergeCell ref="D174:I174"/>
+    <mergeCell ref="J174:K174"/>
+    <mergeCell ref="B161:C161"/>
+    <mergeCell ref="D161:I161"/>
+    <mergeCell ref="J161:K161"/>
+    <mergeCell ref="B162:K162"/>
+    <mergeCell ref="B163:C163"/>
+    <mergeCell ref="D163:E163"/>
+    <mergeCell ref="F163:I163"/>
+    <mergeCell ref="J163:K163"/>
+    <mergeCell ref="B164:C164"/>
+    <mergeCell ref="D164:E164"/>
+    <mergeCell ref="F164:I164"/>
+    <mergeCell ref="J164:K164"/>
+    <mergeCell ref="B152:K152"/>
+    <mergeCell ref="B153:K153"/>
+    <mergeCell ref="B154:K157"/>
+    <mergeCell ref="B158:C158"/>
+    <mergeCell ref="D158:F158"/>
+    <mergeCell ref="G158:H158"/>
+    <mergeCell ref="I158:K158"/>
+    <mergeCell ref="B159:K159"/>
+    <mergeCell ref="B160:K160"/>
+    <mergeCell ref="B91:K91"/>
+    <mergeCell ref="B92:K92"/>
+    <mergeCell ref="B89:C89"/>
+    <mergeCell ref="D89:E89"/>
+    <mergeCell ref="F89:I89"/>
+    <mergeCell ref="J89:K89"/>
+    <mergeCell ref="B90:C90"/>
+    <mergeCell ref="D90:E90"/>
+    <mergeCell ref="F90:I90"/>
+    <mergeCell ref="J90:K90"/>
+    <mergeCell ref="B88:C88"/>
+    <mergeCell ref="D88:E88"/>
+    <mergeCell ref="F88:I88"/>
+    <mergeCell ref="J88:K88"/>
+    <mergeCell ref="B84:C84"/>
+    <mergeCell ref="D84:I84"/>
+    <mergeCell ref="J84:K84"/>
+    <mergeCell ref="B85:K85"/>
+    <mergeCell ref="B86:C86"/>
+    <mergeCell ref="D86:E86"/>
+    <mergeCell ref="F86:I86"/>
+    <mergeCell ref="J86:K86"/>
+    <mergeCell ref="B76:K76"/>
+    <mergeCell ref="B77:K80"/>
+    <mergeCell ref="B81:K81"/>
+    <mergeCell ref="B82:K82"/>
+    <mergeCell ref="B83:C83"/>
+    <mergeCell ref="D83:I83"/>
+    <mergeCell ref="J83:K83"/>
+    <mergeCell ref="B87:C87"/>
+    <mergeCell ref="D87:E87"/>
+    <mergeCell ref="F87:I87"/>
+    <mergeCell ref="J87:K87"/>
+    <mergeCell ref="B31:K31"/>
+    <mergeCell ref="B32:K32"/>
+    <mergeCell ref="B74:K74"/>
+    <mergeCell ref="B75:C75"/>
+    <mergeCell ref="D75:E75"/>
+    <mergeCell ref="F75:I75"/>
+    <mergeCell ref="J75:K75"/>
+    <mergeCell ref="B71:K71"/>
+    <mergeCell ref="B72:K72"/>
+    <mergeCell ref="B73:C73"/>
+    <mergeCell ref="D73:I73"/>
+    <mergeCell ref="J73:K73"/>
+    <mergeCell ref="B51:K51"/>
+    <mergeCell ref="J40:K40"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="J41:K41"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="D53:I53"/>
+    <mergeCell ref="J53:K53"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="F44:I44"/>
+    <mergeCell ref="J44:K44"/>
+    <mergeCell ref="B64:K64"/>
+    <mergeCell ref="B65:K65"/>
+    <mergeCell ref="B66:K69"/>
+    <mergeCell ref="B70:C70"/>
+    <mergeCell ref="D70:F70"/>
+    <mergeCell ref="G70:H70"/>
+    <mergeCell ref="I70:K70"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="D57:E57"/>
+    <mergeCell ref="F57:I57"/>
+    <mergeCell ref="J57:K57"/>
+    <mergeCell ref="B62:K62"/>
+    <mergeCell ref="F59:I59"/>
+    <mergeCell ref="J59:K59"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="D58:E58"/>
+    <mergeCell ref="F58:I58"/>
+    <mergeCell ref="J58:K58"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="D54:I54"/>
+    <mergeCell ref="J54:K54"/>
+    <mergeCell ref="B61:K61"/>
+    <mergeCell ref="B55:K55"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="D56:E56"/>
+    <mergeCell ref="F56:I56"/>
+    <mergeCell ref="J56:K56"/>
+    <mergeCell ref="B60:C60"/>
+    <mergeCell ref="D60:E60"/>
+    <mergeCell ref="F60:I60"/>
+    <mergeCell ref="J60:K60"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="D59:E59"/>
+    <mergeCell ref="D40:I40"/>
+    <mergeCell ref="D41:I41"/>
+    <mergeCell ref="B42:K42"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="G37:H37"/>
+    <mergeCell ref="D37:F37"/>
+    <mergeCell ref="I37:K37"/>
+    <mergeCell ref="B38:K38"/>
+    <mergeCell ref="B39:K39"/>
+    <mergeCell ref="B2:K2"/>
+    <mergeCell ref="B3:K3"/>
+    <mergeCell ref="B4:K28"/>
+    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="E29:K29"/>
+    <mergeCell ref="B94:K94"/>
+    <mergeCell ref="B95:K95"/>
+    <mergeCell ref="B96:K99"/>
+    <mergeCell ref="B100:C100"/>
+    <mergeCell ref="D100:F100"/>
+    <mergeCell ref="G100:H100"/>
+    <mergeCell ref="I100:K100"/>
+    <mergeCell ref="B33:K36"/>
+    <mergeCell ref="B52:K52"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="F43:I43"/>
+    <mergeCell ref="J43:K43"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="F45:I45"/>
+    <mergeCell ref="J45:K45"/>
+    <mergeCell ref="B46:K46"/>
+    <mergeCell ref="B47:K50"/>
+    <mergeCell ref="B112:K112"/>
+    <mergeCell ref="B113:K113"/>
+    <mergeCell ref="B114:C114"/>
+    <mergeCell ref="D114:I114"/>
+    <mergeCell ref="J114:K114"/>
+    <mergeCell ref="B115:C115"/>
+    <mergeCell ref="D115:I115"/>
+    <mergeCell ref="J115:K115"/>
+    <mergeCell ref="B101:K101"/>
+    <mergeCell ref="B102:K102"/>
+    <mergeCell ref="B103:C103"/>
+    <mergeCell ref="D103:I103"/>
+    <mergeCell ref="J103:K103"/>
+    <mergeCell ref="B104:K104"/>
+    <mergeCell ref="B105:C105"/>
+    <mergeCell ref="D105:E105"/>
+    <mergeCell ref="F105:I105"/>
+    <mergeCell ref="J105:K105"/>
     <mergeCell ref="B120:K120"/>
     <mergeCell ref="B121:K121"/>
     <mergeCell ref="B106:C106"/>
@@ -3781,147 +4415,49 @@
     <mergeCell ref="J118:K118"/>
     <mergeCell ref="B107:K107"/>
     <mergeCell ref="B108:K111"/>
-    <mergeCell ref="B112:K112"/>
-    <mergeCell ref="B113:K113"/>
-    <mergeCell ref="B114:C114"/>
-    <mergeCell ref="D114:I114"/>
-    <mergeCell ref="J114:K114"/>
-    <mergeCell ref="B115:C115"/>
-    <mergeCell ref="D115:I115"/>
-    <mergeCell ref="J115:K115"/>
-    <mergeCell ref="B101:K101"/>
-    <mergeCell ref="B102:K102"/>
-    <mergeCell ref="B103:C103"/>
-    <mergeCell ref="D103:I103"/>
-    <mergeCell ref="J103:K103"/>
-    <mergeCell ref="B104:K104"/>
-    <mergeCell ref="B105:C105"/>
-    <mergeCell ref="D105:E105"/>
-    <mergeCell ref="F105:I105"/>
-    <mergeCell ref="J105:K105"/>
-    <mergeCell ref="B2:K2"/>
-    <mergeCell ref="B3:K3"/>
-    <mergeCell ref="B4:K28"/>
-    <mergeCell ref="B29:D29"/>
-    <mergeCell ref="E29:K29"/>
-    <mergeCell ref="B94:K94"/>
-    <mergeCell ref="B95:K95"/>
-    <mergeCell ref="B96:K99"/>
-    <mergeCell ref="B100:C100"/>
-    <mergeCell ref="D100:F100"/>
-    <mergeCell ref="G100:H100"/>
-    <mergeCell ref="I100:K100"/>
-    <mergeCell ref="B33:K36"/>
-    <mergeCell ref="B52:K52"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="F43:I43"/>
-    <mergeCell ref="J43:K43"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="F45:I45"/>
-    <mergeCell ref="J45:K45"/>
-    <mergeCell ref="B46:K46"/>
-    <mergeCell ref="B47:K50"/>
-    <mergeCell ref="D40:I40"/>
-    <mergeCell ref="D41:I41"/>
-    <mergeCell ref="B42:K42"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="G37:H37"/>
-    <mergeCell ref="D37:F37"/>
-    <mergeCell ref="I37:K37"/>
-    <mergeCell ref="B38:K38"/>
-    <mergeCell ref="B39:K39"/>
-    <mergeCell ref="B62:K62"/>
-    <mergeCell ref="F59:I59"/>
-    <mergeCell ref="J59:K59"/>
-    <mergeCell ref="B58:C58"/>
-    <mergeCell ref="D58:E58"/>
-    <mergeCell ref="F58:I58"/>
-    <mergeCell ref="J58:K58"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="D54:I54"/>
-    <mergeCell ref="J54:K54"/>
-    <mergeCell ref="B61:K61"/>
-    <mergeCell ref="B55:K55"/>
-    <mergeCell ref="B56:C56"/>
-    <mergeCell ref="D56:E56"/>
-    <mergeCell ref="F56:I56"/>
-    <mergeCell ref="J56:K56"/>
-    <mergeCell ref="B60:C60"/>
-    <mergeCell ref="D60:E60"/>
-    <mergeCell ref="F60:I60"/>
-    <mergeCell ref="J60:K60"/>
-    <mergeCell ref="B59:C59"/>
-    <mergeCell ref="D59:E59"/>
-    <mergeCell ref="B64:K64"/>
-    <mergeCell ref="B65:K65"/>
-    <mergeCell ref="B66:K69"/>
-    <mergeCell ref="B70:C70"/>
-    <mergeCell ref="D70:F70"/>
-    <mergeCell ref="G70:H70"/>
-    <mergeCell ref="I70:K70"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="D57:E57"/>
-    <mergeCell ref="F57:I57"/>
-    <mergeCell ref="J57:K57"/>
-    <mergeCell ref="B51:K51"/>
-    <mergeCell ref="J40:K40"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="J41:K41"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="D53:I53"/>
-    <mergeCell ref="J53:K53"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="F44:I44"/>
-    <mergeCell ref="J44:K44"/>
-    <mergeCell ref="B31:K31"/>
-    <mergeCell ref="B32:K32"/>
-    <mergeCell ref="B74:K74"/>
-    <mergeCell ref="B75:C75"/>
-    <mergeCell ref="D75:E75"/>
-    <mergeCell ref="F75:I75"/>
-    <mergeCell ref="J75:K75"/>
-    <mergeCell ref="B71:K71"/>
-    <mergeCell ref="B72:K72"/>
-    <mergeCell ref="B73:C73"/>
-    <mergeCell ref="D73:I73"/>
-    <mergeCell ref="J73:K73"/>
-    <mergeCell ref="B76:K76"/>
-    <mergeCell ref="B77:K80"/>
-    <mergeCell ref="B81:K81"/>
-    <mergeCell ref="B82:K82"/>
-    <mergeCell ref="B83:C83"/>
-    <mergeCell ref="D83:I83"/>
-    <mergeCell ref="J83:K83"/>
-    <mergeCell ref="B87:C87"/>
-    <mergeCell ref="D87:E87"/>
-    <mergeCell ref="F87:I87"/>
-    <mergeCell ref="J87:K87"/>
-    <mergeCell ref="B88:C88"/>
-    <mergeCell ref="D88:E88"/>
-    <mergeCell ref="F88:I88"/>
-    <mergeCell ref="J88:K88"/>
-    <mergeCell ref="B84:C84"/>
-    <mergeCell ref="D84:I84"/>
-    <mergeCell ref="J84:K84"/>
-    <mergeCell ref="B85:K85"/>
-    <mergeCell ref="B86:C86"/>
-    <mergeCell ref="D86:E86"/>
-    <mergeCell ref="F86:I86"/>
-    <mergeCell ref="J86:K86"/>
-    <mergeCell ref="B91:K91"/>
-    <mergeCell ref="B92:K92"/>
-    <mergeCell ref="B89:C89"/>
-    <mergeCell ref="D89:E89"/>
-    <mergeCell ref="F89:I89"/>
-    <mergeCell ref="J89:K89"/>
-    <mergeCell ref="B90:C90"/>
-    <mergeCell ref="D90:E90"/>
-    <mergeCell ref="F90:I90"/>
-    <mergeCell ref="J90:K90"/>
+    <mergeCell ref="B129:C129"/>
+    <mergeCell ref="D129:F129"/>
+    <mergeCell ref="G129:H129"/>
+    <mergeCell ref="I129:K129"/>
+    <mergeCell ref="B130:K130"/>
+    <mergeCell ref="B131:K131"/>
+    <mergeCell ref="B132:C132"/>
+    <mergeCell ref="D132:I132"/>
+    <mergeCell ref="J132:K132"/>
+    <mergeCell ref="B133:K133"/>
+    <mergeCell ref="B134:C134"/>
+    <mergeCell ref="D134:E134"/>
+    <mergeCell ref="F134:I134"/>
+    <mergeCell ref="J134:K134"/>
+    <mergeCell ref="B135:C135"/>
+    <mergeCell ref="D135:E135"/>
+    <mergeCell ref="F135:I135"/>
+    <mergeCell ref="J135:K135"/>
+    <mergeCell ref="B136:K136"/>
+    <mergeCell ref="B137:K140"/>
+    <mergeCell ref="B141:K141"/>
+    <mergeCell ref="B142:K142"/>
+    <mergeCell ref="B143:C143"/>
+    <mergeCell ref="D143:I143"/>
+    <mergeCell ref="J143:K143"/>
+    <mergeCell ref="B144:C144"/>
+    <mergeCell ref="D144:I144"/>
+    <mergeCell ref="J144:K144"/>
+    <mergeCell ref="B148:C148"/>
+    <mergeCell ref="D148:E148"/>
+    <mergeCell ref="F148:I148"/>
+    <mergeCell ref="J148:K148"/>
+    <mergeCell ref="B149:K149"/>
+    <mergeCell ref="B150:K150"/>
+    <mergeCell ref="B145:K145"/>
+    <mergeCell ref="B146:C146"/>
+    <mergeCell ref="D146:E146"/>
+    <mergeCell ref="F146:I146"/>
+    <mergeCell ref="J146:K146"/>
+    <mergeCell ref="B147:C147"/>
+    <mergeCell ref="D147:E147"/>
+    <mergeCell ref="F147:I147"/>
+    <mergeCell ref="J147:K147"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
240423 16:50 Update front back
</commit_message>
<xml_diff>
--- a/API 명세서.xlsx
+++ b/API 명세서.xlsx
@@ -1169,6 +1169,18 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1199,18 +1211,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1337,59 +1337,59 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1673,367 +1673,367 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:L212"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A193" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A206" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="B212" sqref="B212:K212"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="2" spans="2:12" ht="54" x14ac:dyDescent="0.3">
-      <c r="B2" s="61" t="s">
+      <c r="B2" s="60" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="62"/>
-      <c r="D2" s="62"/>
-      <c r="E2" s="62"/>
-      <c r="F2" s="62"/>
-      <c r="G2" s="62"/>
-      <c r="H2" s="62"/>
-      <c r="I2" s="62"/>
-      <c r="J2" s="62"/>
-      <c r="K2" s="63"/>
+      <c r="C2" s="61"/>
+      <c r="D2" s="61"/>
+      <c r="E2" s="61"/>
+      <c r="F2" s="61"/>
+      <c r="G2" s="61"/>
+      <c r="H2" s="61"/>
+      <c r="I2" s="61"/>
+      <c r="J2" s="61"/>
+      <c r="K2" s="62"/>
       <c r="L2" s="1"/>
     </row>
     <row r="3" spans="2:12" ht="31.5" x14ac:dyDescent="0.3">
-      <c r="B3" s="64" t="s">
+      <c r="B3" s="63" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="65"/>
-      <c r="D3" s="65"/>
-      <c r="E3" s="65"/>
-      <c r="F3" s="65"/>
-      <c r="G3" s="65"/>
-      <c r="H3" s="65"/>
-      <c r="I3" s="65"/>
-      <c r="J3" s="65"/>
-      <c r="K3" s="66"/>
+      <c r="C3" s="64"/>
+      <c r="D3" s="64"/>
+      <c r="E3" s="64"/>
+      <c r="F3" s="64"/>
+      <c r="G3" s="64"/>
+      <c r="H3" s="64"/>
+      <c r="I3" s="64"/>
+      <c r="J3" s="64"/>
+      <c r="K3" s="65"/>
       <c r="L3" s="2"/>
     </row>
     <row r="4" spans="2:12" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="67" t="s">
+      <c r="B4" s="66" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="68"/>
-      <c r="D4" s="68"/>
-      <c r="E4" s="68"/>
-      <c r="F4" s="68"/>
-      <c r="G4" s="68"/>
-      <c r="H4" s="68"/>
-      <c r="I4" s="68"/>
-      <c r="J4" s="68"/>
-      <c r="K4" s="69"/>
+      <c r="C4" s="67"/>
+      <c r="D4" s="67"/>
+      <c r="E4" s="67"/>
+      <c r="F4" s="67"/>
+      <c r="G4" s="67"/>
+      <c r="H4" s="67"/>
+      <c r="I4" s="67"/>
+      <c r="J4" s="67"/>
+      <c r="K4" s="68"/>
       <c r="L4" s="3"/>
     </row>
     <row r="5" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="70"/>
-      <c r="C5" s="71"/>
-      <c r="D5" s="71"/>
-      <c r="E5" s="71"/>
-      <c r="F5" s="71"/>
-      <c r="G5" s="71"/>
-      <c r="H5" s="71"/>
-      <c r="I5" s="71"/>
-      <c r="J5" s="71"/>
-      <c r="K5" s="72"/>
+      <c r="B5" s="69"/>
+      <c r="C5" s="70"/>
+      <c r="D5" s="70"/>
+      <c r="E5" s="70"/>
+      <c r="F5" s="70"/>
+      <c r="G5" s="70"/>
+      <c r="H5" s="70"/>
+      <c r="I5" s="70"/>
+      <c r="J5" s="70"/>
+      <c r="K5" s="71"/>
       <c r="L5" s="3"/>
     </row>
     <row r="6" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="70"/>
-      <c r="C6" s="71"/>
-      <c r="D6" s="71"/>
-      <c r="E6" s="71"/>
-      <c r="F6" s="71"/>
-      <c r="G6" s="71"/>
-      <c r="H6" s="71"/>
-      <c r="I6" s="71"/>
-      <c r="J6" s="71"/>
-      <c r="K6" s="72"/>
+      <c r="B6" s="69"/>
+      <c r="C6" s="70"/>
+      <c r="D6" s="70"/>
+      <c r="E6" s="70"/>
+      <c r="F6" s="70"/>
+      <c r="G6" s="70"/>
+      <c r="H6" s="70"/>
+      <c r="I6" s="70"/>
+      <c r="J6" s="70"/>
+      <c r="K6" s="71"/>
       <c r="L6" s="3"/>
     </row>
     <row r="7" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="70"/>
-      <c r="C7" s="71"/>
-      <c r="D7" s="71"/>
-      <c r="E7" s="71"/>
-      <c r="F7" s="71"/>
-      <c r="G7" s="71"/>
-      <c r="H7" s="71"/>
-      <c r="I7" s="71"/>
-      <c r="J7" s="71"/>
-      <c r="K7" s="72"/>
+      <c r="B7" s="69"/>
+      <c r="C7" s="70"/>
+      <c r="D7" s="70"/>
+      <c r="E7" s="70"/>
+      <c r="F7" s="70"/>
+      <c r="G7" s="70"/>
+      <c r="H7" s="70"/>
+      <c r="I7" s="70"/>
+      <c r="J7" s="70"/>
+      <c r="K7" s="71"/>
       <c r="L7" s="3"/>
     </row>
     <row r="8" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="70"/>
-      <c r="C8" s="71"/>
-      <c r="D8" s="71"/>
-      <c r="E8" s="71"/>
-      <c r="F8" s="71"/>
-      <c r="G8" s="71"/>
-      <c r="H8" s="71"/>
-      <c r="I8" s="71"/>
-      <c r="J8" s="71"/>
-      <c r="K8" s="72"/>
+      <c r="B8" s="69"/>
+      <c r="C8" s="70"/>
+      <c r="D8" s="70"/>
+      <c r="E8" s="70"/>
+      <c r="F8" s="70"/>
+      <c r="G8" s="70"/>
+      <c r="H8" s="70"/>
+      <c r="I8" s="70"/>
+      <c r="J8" s="70"/>
+      <c r="K8" s="71"/>
       <c r="L8" s="3"/>
     </row>
     <row r="9" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="70"/>
-      <c r="C9" s="71"/>
-      <c r="D9" s="71"/>
-      <c r="E9" s="71"/>
-      <c r="F9" s="71"/>
-      <c r="G9" s="71"/>
-      <c r="H9" s="71"/>
-      <c r="I9" s="71"/>
-      <c r="J9" s="71"/>
-      <c r="K9" s="72"/>
+      <c r="B9" s="69"/>
+      <c r="C9" s="70"/>
+      <c r="D9" s="70"/>
+      <c r="E9" s="70"/>
+      <c r="F9" s="70"/>
+      <c r="G9" s="70"/>
+      <c r="H9" s="70"/>
+      <c r="I9" s="70"/>
+      <c r="J9" s="70"/>
+      <c r="K9" s="71"/>
       <c r="L9" s="3"/>
     </row>
     <row r="10" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="70"/>
-      <c r="C10" s="71"/>
-      <c r="D10" s="71"/>
-      <c r="E10" s="71"/>
-      <c r="F10" s="71"/>
-      <c r="G10" s="71"/>
-      <c r="H10" s="71"/>
-      <c r="I10" s="71"/>
-      <c r="J10" s="71"/>
-      <c r="K10" s="72"/>
+      <c r="B10" s="69"/>
+      <c r="C10" s="70"/>
+      <c r="D10" s="70"/>
+      <c r="E10" s="70"/>
+      <c r="F10" s="70"/>
+      <c r="G10" s="70"/>
+      <c r="H10" s="70"/>
+      <c r="I10" s="70"/>
+      <c r="J10" s="70"/>
+      <c r="K10" s="71"/>
       <c r="L10" s="3"/>
     </row>
     <row r="11" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="70"/>
-      <c r="C11" s="71"/>
-      <c r="D11" s="71"/>
-      <c r="E11" s="71"/>
-      <c r="F11" s="71"/>
-      <c r="G11" s="71"/>
-      <c r="H11" s="71"/>
-      <c r="I11" s="71"/>
-      <c r="J11" s="71"/>
-      <c r="K11" s="72"/>
+      <c r="B11" s="69"/>
+      <c r="C11" s="70"/>
+      <c r="D11" s="70"/>
+      <c r="E11" s="70"/>
+      <c r="F11" s="70"/>
+      <c r="G11" s="70"/>
+      <c r="H11" s="70"/>
+      <c r="I11" s="70"/>
+      <c r="J11" s="70"/>
+      <c r="K11" s="71"/>
       <c r="L11" s="3"/>
     </row>
     <row r="12" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="70"/>
-      <c r="C12" s="71"/>
-      <c r="D12" s="71"/>
-      <c r="E12" s="71"/>
-      <c r="F12" s="71"/>
-      <c r="G12" s="71"/>
-      <c r="H12" s="71"/>
-      <c r="I12" s="71"/>
-      <c r="J12" s="71"/>
-      <c r="K12" s="72"/>
+      <c r="B12" s="69"/>
+      <c r="C12" s="70"/>
+      <c r="D12" s="70"/>
+      <c r="E12" s="70"/>
+      <c r="F12" s="70"/>
+      <c r="G12" s="70"/>
+      <c r="H12" s="70"/>
+      <c r="I12" s="70"/>
+      <c r="J12" s="70"/>
+      <c r="K12" s="71"/>
       <c r="L12" s="3"/>
     </row>
     <row r="13" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="70"/>
-      <c r="C13" s="71"/>
-      <c r="D13" s="71"/>
-      <c r="E13" s="71"/>
-      <c r="F13" s="71"/>
-      <c r="G13" s="71"/>
-      <c r="H13" s="71"/>
-      <c r="I13" s="71"/>
-      <c r="J13" s="71"/>
-      <c r="K13" s="72"/>
+      <c r="B13" s="69"/>
+      <c r="C13" s="70"/>
+      <c r="D13" s="70"/>
+      <c r="E13" s="70"/>
+      <c r="F13" s="70"/>
+      <c r="G13" s="70"/>
+      <c r="H13" s="70"/>
+      <c r="I13" s="70"/>
+      <c r="J13" s="70"/>
+      <c r="K13" s="71"/>
       <c r="L13" s="3"/>
     </row>
     <row r="14" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="70"/>
-      <c r="C14" s="71"/>
-      <c r="D14" s="71"/>
-      <c r="E14" s="71"/>
-      <c r="F14" s="71"/>
-      <c r="G14" s="71"/>
-      <c r="H14" s="71"/>
-      <c r="I14" s="71"/>
-      <c r="J14" s="71"/>
-      <c r="K14" s="72"/>
+      <c r="B14" s="69"/>
+      <c r="C14" s="70"/>
+      <c r="D14" s="70"/>
+      <c r="E14" s="70"/>
+      <c r="F14" s="70"/>
+      <c r="G14" s="70"/>
+      <c r="H14" s="70"/>
+      <c r="I14" s="70"/>
+      <c r="J14" s="70"/>
+      <c r="K14" s="71"/>
       <c r="L14" s="3"/>
     </row>
     <row r="15" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="70"/>
-      <c r="C15" s="71"/>
-      <c r="D15" s="71"/>
-      <c r="E15" s="71"/>
-      <c r="F15" s="71"/>
-      <c r="G15" s="71"/>
-      <c r="H15" s="71"/>
-      <c r="I15" s="71"/>
-      <c r="J15" s="71"/>
-      <c r="K15" s="72"/>
+      <c r="B15" s="69"/>
+      <c r="C15" s="70"/>
+      <c r="D15" s="70"/>
+      <c r="E15" s="70"/>
+      <c r="F15" s="70"/>
+      <c r="G15" s="70"/>
+      <c r="H15" s="70"/>
+      <c r="I15" s="70"/>
+      <c r="J15" s="70"/>
+      <c r="K15" s="71"/>
       <c r="L15" s="3"/>
     </row>
     <row r="16" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="70"/>
-      <c r="C16" s="71"/>
-      <c r="D16" s="71"/>
-      <c r="E16" s="71"/>
-      <c r="F16" s="71"/>
-      <c r="G16" s="71"/>
-      <c r="H16" s="71"/>
-      <c r="I16" s="71"/>
-      <c r="J16" s="71"/>
-      <c r="K16" s="72"/>
+      <c r="B16" s="69"/>
+      <c r="C16" s="70"/>
+      <c r="D16" s="70"/>
+      <c r="E16" s="70"/>
+      <c r="F16" s="70"/>
+      <c r="G16" s="70"/>
+      <c r="H16" s="70"/>
+      <c r="I16" s="70"/>
+      <c r="J16" s="70"/>
+      <c r="K16" s="71"/>
       <c r="L16" s="3"/>
     </row>
     <row r="17" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="70"/>
-      <c r="C17" s="71"/>
-      <c r="D17" s="71"/>
-      <c r="E17" s="71"/>
-      <c r="F17" s="71"/>
-      <c r="G17" s="71"/>
-      <c r="H17" s="71"/>
-      <c r="I17" s="71"/>
-      <c r="J17" s="71"/>
-      <c r="K17" s="72"/>
+      <c r="B17" s="69"/>
+      <c r="C17" s="70"/>
+      <c r="D17" s="70"/>
+      <c r="E17" s="70"/>
+      <c r="F17" s="70"/>
+      <c r="G17" s="70"/>
+      <c r="H17" s="70"/>
+      <c r="I17" s="70"/>
+      <c r="J17" s="70"/>
+      <c r="K17" s="71"/>
       <c r="L17" s="3"/>
     </row>
     <row r="18" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="70"/>
-      <c r="C18" s="71"/>
-      <c r="D18" s="71"/>
-      <c r="E18" s="71"/>
-      <c r="F18" s="71"/>
-      <c r="G18" s="71"/>
-      <c r="H18" s="71"/>
-      <c r="I18" s="71"/>
-      <c r="J18" s="71"/>
-      <c r="K18" s="72"/>
+      <c r="B18" s="69"/>
+      <c r="C18" s="70"/>
+      <c r="D18" s="70"/>
+      <c r="E18" s="70"/>
+      <c r="F18" s="70"/>
+      <c r="G18" s="70"/>
+      <c r="H18" s="70"/>
+      <c r="I18" s="70"/>
+      <c r="J18" s="70"/>
+      <c r="K18" s="71"/>
       <c r="L18" s="3"/>
     </row>
     <row r="19" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="70"/>
-      <c r="C19" s="71"/>
-      <c r="D19" s="71"/>
-      <c r="E19" s="71"/>
-      <c r="F19" s="71"/>
-      <c r="G19" s="71"/>
-      <c r="H19" s="71"/>
-      <c r="I19" s="71"/>
-      <c r="J19" s="71"/>
-      <c r="K19" s="72"/>
+      <c r="B19" s="69"/>
+      <c r="C19" s="70"/>
+      <c r="D19" s="70"/>
+      <c r="E19" s="70"/>
+      <c r="F19" s="70"/>
+      <c r="G19" s="70"/>
+      <c r="H19" s="70"/>
+      <c r="I19" s="70"/>
+      <c r="J19" s="70"/>
+      <c r="K19" s="71"/>
       <c r="L19" s="3"/>
     </row>
     <row r="20" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="70"/>
-      <c r="C20" s="71"/>
-      <c r="D20" s="71"/>
-      <c r="E20" s="71"/>
-      <c r="F20" s="71"/>
-      <c r="G20" s="71"/>
-      <c r="H20" s="71"/>
-      <c r="I20" s="71"/>
-      <c r="J20" s="71"/>
-      <c r="K20" s="72"/>
+      <c r="B20" s="69"/>
+      <c r="C20" s="70"/>
+      <c r="D20" s="70"/>
+      <c r="E20" s="70"/>
+      <c r="F20" s="70"/>
+      <c r="G20" s="70"/>
+      <c r="H20" s="70"/>
+      <c r="I20" s="70"/>
+      <c r="J20" s="70"/>
+      <c r="K20" s="71"/>
       <c r="L20" s="3"/>
     </row>
     <row r="21" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="70"/>
-      <c r="C21" s="71"/>
-      <c r="D21" s="71"/>
-      <c r="E21" s="71"/>
-      <c r="F21" s="71"/>
-      <c r="G21" s="71"/>
-      <c r="H21" s="71"/>
-      <c r="I21" s="71"/>
-      <c r="J21" s="71"/>
-      <c r="K21" s="72"/>
+      <c r="B21" s="69"/>
+      <c r="C21" s="70"/>
+      <c r="D21" s="70"/>
+      <c r="E21" s="70"/>
+      <c r="F21" s="70"/>
+      <c r="G21" s="70"/>
+      <c r="H21" s="70"/>
+      <c r="I21" s="70"/>
+      <c r="J21" s="70"/>
+      <c r="K21" s="71"/>
       <c r="L21" s="3"/>
     </row>
     <row r="22" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="70"/>
-      <c r="C22" s="71"/>
-      <c r="D22" s="71"/>
-      <c r="E22" s="71"/>
-      <c r="F22" s="71"/>
-      <c r="G22" s="71"/>
-      <c r="H22" s="71"/>
-      <c r="I22" s="71"/>
-      <c r="J22" s="71"/>
-      <c r="K22" s="72"/>
+      <c r="B22" s="69"/>
+      <c r="C22" s="70"/>
+      <c r="D22" s="70"/>
+      <c r="E22" s="70"/>
+      <c r="F22" s="70"/>
+      <c r="G22" s="70"/>
+      <c r="H22" s="70"/>
+      <c r="I22" s="70"/>
+      <c r="J22" s="70"/>
+      <c r="K22" s="71"/>
       <c r="L22" s="3"/>
     </row>
     <row r="23" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="70"/>
-      <c r="C23" s="71"/>
-      <c r="D23" s="71"/>
-      <c r="E23" s="71"/>
-      <c r="F23" s="71"/>
-      <c r="G23" s="71"/>
-      <c r="H23" s="71"/>
-      <c r="I23" s="71"/>
-      <c r="J23" s="71"/>
-      <c r="K23" s="72"/>
+      <c r="B23" s="69"/>
+      <c r="C23" s="70"/>
+      <c r="D23" s="70"/>
+      <c r="E23" s="70"/>
+      <c r="F23" s="70"/>
+      <c r="G23" s="70"/>
+      <c r="H23" s="70"/>
+      <c r="I23" s="70"/>
+      <c r="J23" s="70"/>
+      <c r="K23" s="71"/>
       <c r="L23" s="3"/>
     </row>
     <row r="24" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="70"/>
-      <c r="C24" s="71"/>
-      <c r="D24" s="71"/>
-      <c r="E24" s="71"/>
-      <c r="F24" s="71"/>
-      <c r="G24" s="71"/>
-      <c r="H24" s="71"/>
-      <c r="I24" s="71"/>
-      <c r="J24" s="71"/>
-      <c r="K24" s="72"/>
+      <c r="B24" s="69"/>
+      <c r="C24" s="70"/>
+      <c r="D24" s="70"/>
+      <c r="E24" s="70"/>
+      <c r="F24" s="70"/>
+      <c r="G24" s="70"/>
+      <c r="H24" s="70"/>
+      <c r="I24" s="70"/>
+      <c r="J24" s="70"/>
+      <c r="K24" s="71"/>
       <c r="L24" s="3"/>
     </row>
     <row r="25" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="70"/>
-      <c r="C25" s="71"/>
-      <c r="D25" s="71"/>
-      <c r="E25" s="71"/>
-      <c r="F25" s="71"/>
-      <c r="G25" s="71"/>
-      <c r="H25" s="71"/>
-      <c r="I25" s="71"/>
-      <c r="J25" s="71"/>
-      <c r="K25" s="72"/>
+      <c r="B25" s="69"/>
+      <c r="C25" s="70"/>
+      <c r="D25" s="70"/>
+      <c r="E25" s="70"/>
+      <c r="F25" s="70"/>
+      <c r="G25" s="70"/>
+      <c r="H25" s="70"/>
+      <c r="I25" s="70"/>
+      <c r="J25" s="70"/>
+      <c r="K25" s="71"/>
       <c r="L25" s="3"/>
     </row>
     <row r="26" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="70"/>
-      <c r="C26" s="71"/>
-      <c r="D26" s="71"/>
-      <c r="E26" s="71"/>
-      <c r="F26" s="71"/>
-      <c r="G26" s="71"/>
-      <c r="H26" s="71"/>
-      <c r="I26" s="71"/>
-      <c r="J26" s="71"/>
-      <c r="K26" s="72"/>
+      <c r="B26" s="69"/>
+      <c r="C26" s="70"/>
+      <c r="D26" s="70"/>
+      <c r="E26" s="70"/>
+      <c r="F26" s="70"/>
+      <c r="G26" s="70"/>
+      <c r="H26" s="70"/>
+      <c r="I26" s="70"/>
+      <c r="J26" s="70"/>
+      <c r="K26" s="71"/>
       <c r="L26" s="3"/>
     </row>
     <row r="27" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="70"/>
-      <c r="C27" s="71"/>
-      <c r="D27" s="71"/>
-      <c r="E27" s="71"/>
-      <c r="F27" s="71"/>
-      <c r="G27" s="71"/>
-      <c r="H27" s="71"/>
-      <c r="I27" s="71"/>
-      <c r="J27" s="71"/>
-      <c r="K27" s="72"/>
+      <c r="B27" s="69"/>
+      <c r="C27" s="70"/>
+      <c r="D27" s="70"/>
+      <c r="E27" s="70"/>
+      <c r="F27" s="70"/>
+      <c r="G27" s="70"/>
+      <c r="H27" s="70"/>
+      <c r="I27" s="70"/>
+      <c r="J27" s="70"/>
+      <c r="K27" s="71"/>
       <c r="L27" s="3"/>
     </row>
     <row r="28" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="73"/>
-      <c r="C28" s="74"/>
-      <c r="D28" s="74"/>
-      <c r="E28" s="74"/>
-      <c r="F28" s="74"/>
-      <c r="G28" s="74"/>
-      <c r="H28" s="74"/>
-      <c r="I28" s="74"/>
-      <c r="J28" s="74"/>
-      <c r="K28" s="75"/>
+      <c r="B28" s="72"/>
+      <c r="C28" s="73"/>
+      <c r="D28" s="73"/>
+      <c r="E28" s="73"/>
+      <c r="F28" s="73"/>
+      <c r="G28" s="73"/>
+      <c r="H28" s="73"/>
+      <c r="I28" s="73"/>
+      <c r="J28" s="73"/>
+      <c r="K28" s="74"/>
       <c r="L28" s="3"/>
     </row>
     <row r="29" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -2042,15 +2042,15 @@
       </c>
       <c r="C29" s="45"/>
       <c r="D29" s="45"/>
-      <c r="E29" s="76" t="s">
+      <c r="E29" s="75" t="s">
         <v>20</v>
       </c>
-      <c r="F29" s="76"/>
-      <c r="G29" s="76"/>
-      <c r="H29" s="76"/>
-      <c r="I29" s="76"/>
-      <c r="J29" s="76"/>
-      <c r="K29" s="77"/>
+      <c r="F29" s="75"/>
+      <c r="G29" s="75"/>
+      <c r="H29" s="75"/>
+      <c r="I29" s="75"/>
+      <c r="J29" s="75"/>
+      <c r="K29" s="76"/>
       <c r="L29" s="3"/>
     </row>
     <row r="30" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
@@ -2199,19 +2199,19 @@
       <c r="K40" s="20"/>
     </row>
     <row r="41" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B41" s="4"/>
-      <c r="C41" s="5"/>
-      <c r="D41" s="5"/>
-      <c r="E41" s="5"/>
-      <c r="F41" s="5"/>
-      <c r="G41" s="5"/>
-      <c r="H41" s="5"/>
-      <c r="I41" s="5"/>
-      <c r="J41" s="5"/>
-      <c r="K41" s="7"/>
+      <c r="B41" s="8"/>
+      <c r="C41" s="9"/>
+      <c r="D41" s="9"/>
+      <c r="E41" s="9"/>
+      <c r="F41" s="9"/>
+      <c r="G41" s="9"/>
+      <c r="H41" s="9"/>
+      <c r="I41" s="9"/>
+      <c r="J41" s="9"/>
+      <c r="K41" s="11"/>
     </row>
     <row r="42" spans="2:11" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="B42" s="8" t="s">
+      <c r="B42" s="12" t="s">
         <v>11</v>
       </c>
       <c r="C42" s="21"/>
@@ -2245,47 +2245,47 @@
       <c r="K43" s="20"/>
     </row>
     <row r="44" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B44" s="4" t="s">
+      <c r="B44" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C44" s="5"/>
-      <c r="D44" s="5" t="s">
+      <c r="C44" s="9"/>
+      <c r="D44" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="E44" s="60"/>
-      <c r="F44" s="5" t="s">
+      <c r="E44" s="77"/>
+      <c r="F44" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="G44" s="5"/>
-      <c r="H44" s="5"/>
-      <c r="I44" s="5"/>
-      <c r="J44" s="6" t="s">
+      <c r="G44" s="9"/>
+      <c r="H44" s="9"/>
+      <c r="I44" s="9"/>
+      <c r="J44" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="K44" s="7"/>
+      <c r="K44" s="11"/>
     </row>
     <row r="45" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B45" s="4" t="s">
+      <c r="B45" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="C45" s="5"/>
-      <c r="D45" s="5" t="s">
+      <c r="C45" s="9"/>
+      <c r="D45" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="E45" s="5"/>
-      <c r="F45" s="5" t="s">
+      <c r="E45" s="9"/>
+      <c r="F45" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="G45" s="5"/>
-      <c r="H45" s="5"/>
-      <c r="I45" s="5"/>
-      <c r="J45" s="6" t="s">
+      <c r="G45" s="9"/>
+      <c r="H45" s="9"/>
+      <c r="I45" s="9"/>
+      <c r="J45" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="K45" s="7"/>
+      <c r="K45" s="11"/>
     </row>
     <row r="46" spans="2:11" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="B46" s="8" t="s">
+      <c r="B46" s="12" t="s">
         <v>10</v>
       </c>
       <c r="C46" s="21"/>
@@ -2395,36 +2395,36 @@
       <c r="K53" s="20"/>
     </row>
     <row r="54" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B54" s="4" t="s">
+      <c r="B54" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="C54" s="5"/>
-      <c r="D54" s="5" t="s">
+      <c r="C54" s="9"/>
+      <c r="D54" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="E54" s="5"/>
-      <c r="F54" s="5"/>
-      <c r="G54" s="5"/>
-      <c r="H54" s="5"/>
-      <c r="I54" s="5"/>
-      <c r="J54" s="6" t="s">
+      <c r="E54" s="9"/>
+      <c r="F54" s="9"/>
+      <c r="G54" s="9"/>
+      <c r="H54" s="9"/>
+      <c r="I54" s="9"/>
+      <c r="J54" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="K54" s="7"/>
+      <c r="K54" s="11"/>
     </row>
     <row r="55" spans="2:11" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="B55" s="8" t="s">
+      <c r="B55" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C55" s="9"/>
-      <c r="D55" s="9"/>
-      <c r="E55" s="9"/>
-      <c r="F55" s="9"/>
-      <c r="G55" s="9"/>
-      <c r="H55" s="9"/>
-      <c r="I55" s="9"/>
-      <c r="J55" s="9"/>
-      <c r="K55" s="10"/>
+      <c r="C55" s="13"/>
+      <c r="D55" s="13"/>
+      <c r="E55" s="13"/>
+      <c r="F55" s="13"/>
+      <c r="G55" s="13"/>
+      <c r="H55" s="13"/>
+      <c r="I55" s="13"/>
+      <c r="J55" s="13"/>
+      <c r="K55" s="14"/>
     </row>
     <row r="56" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B56" s="18" t="s">
@@ -2447,112 +2447,112 @@
       <c r="K56" s="20"/>
     </row>
     <row r="57" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B57" s="4" t="s">
+      <c r="B57" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="C57" s="5"/>
-      <c r="D57" s="5" t="s">
+      <c r="C57" s="9"/>
+      <c r="D57" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="E57" s="5"/>
-      <c r="F57" s="5" t="s">
+      <c r="E57" s="9"/>
+      <c r="F57" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="G57" s="5"/>
-      <c r="H57" s="5"/>
-      <c r="I57" s="5"/>
-      <c r="J57" s="6" t="s">
+      <c r="G57" s="9"/>
+      <c r="H57" s="9"/>
+      <c r="I57" s="9"/>
+      <c r="J57" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="K57" s="7"/>
+      <c r="K57" s="11"/>
     </row>
     <row r="58" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B58" s="4" t="s">
+      <c r="B58" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="C58" s="5"/>
-      <c r="D58" s="5" t="s">
+      <c r="C58" s="9"/>
+      <c r="D58" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="E58" s="5"/>
-      <c r="F58" s="5" t="s">
+      <c r="E58" s="9"/>
+      <c r="F58" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="G58" s="5"/>
-      <c r="H58" s="5"/>
-      <c r="I58" s="5"/>
-      <c r="J58" s="6" t="s">
+      <c r="G58" s="9"/>
+      <c r="H58" s="9"/>
+      <c r="I58" s="9"/>
+      <c r="J58" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="K58" s="7"/>
+      <c r="K58" s="11"/>
     </row>
     <row r="59" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B59" s="4" t="s">
+      <c r="B59" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C59" s="5"/>
-      <c r="D59" s="5" t="s">
+      <c r="C59" s="9"/>
+      <c r="D59" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="E59" s="5"/>
-      <c r="F59" s="5" t="s">
+      <c r="E59" s="9"/>
+      <c r="F59" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="G59" s="5"/>
-      <c r="H59" s="5"/>
-      <c r="I59" s="5"/>
-      <c r="J59" s="6" t="s">
+      <c r="G59" s="9"/>
+      <c r="H59" s="9"/>
+      <c r="I59" s="9"/>
+      <c r="J59" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="K59" s="7"/>
+      <c r="K59" s="11"/>
     </row>
     <row r="60" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B60" s="4" t="s">
+      <c r="B60" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="C60" s="5"/>
-      <c r="D60" s="5" t="s">
+      <c r="C60" s="9"/>
+      <c r="D60" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="E60" s="5"/>
-      <c r="F60" s="5" t="s">
+      <c r="E60" s="9"/>
+      <c r="F60" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="G60" s="5"/>
-      <c r="H60" s="5"/>
-      <c r="I60" s="5"/>
-      <c r="J60" s="6" t="s">
+      <c r="G60" s="9"/>
+      <c r="H60" s="9"/>
+      <c r="I60" s="9"/>
+      <c r="J60" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="K60" s="7"/>
+      <c r="K60" s="11"/>
     </row>
     <row r="61" spans="2:11" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="B61" s="8" t="s">
+      <c r="B61" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="C61" s="9"/>
-      <c r="D61" s="9"/>
-      <c r="E61" s="9"/>
-      <c r="F61" s="9"/>
-      <c r="G61" s="9"/>
-      <c r="H61" s="9"/>
-      <c r="I61" s="9"/>
-      <c r="J61" s="9"/>
-      <c r="K61" s="10"/>
+      <c r="C61" s="13"/>
+      <c r="D61" s="13"/>
+      <c r="E61" s="13"/>
+      <c r="F61" s="13"/>
+      <c r="G61" s="13"/>
+      <c r="H61" s="13"/>
+      <c r="I61" s="13"/>
+      <c r="J61" s="13"/>
+      <c r="K61" s="14"/>
     </row>
     <row r="62" spans="2:11" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B62" s="11" t="s">
+      <c r="B62" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="C62" s="12"/>
-      <c r="D62" s="12"/>
-      <c r="E62" s="12"/>
-      <c r="F62" s="12"/>
-      <c r="G62" s="12"/>
-      <c r="H62" s="12"/>
-      <c r="I62" s="12"/>
-      <c r="J62" s="12"/>
-      <c r="K62" s="13"/>
+      <c r="C62" s="16"/>
+      <c r="D62" s="16"/>
+      <c r="E62" s="16"/>
+      <c r="F62" s="16"/>
+      <c r="G62" s="16"/>
+      <c r="H62" s="16"/>
+      <c r="I62" s="16"/>
+      <c r="J62" s="16"/>
+      <c r="K62" s="17"/>
     </row>
     <row r="63" spans="2:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="64" spans="2:11" ht="41.25" x14ac:dyDescent="0.3">
@@ -2700,7 +2700,7 @@
       <c r="K73" s="40"/>
     </row>
     <row r="74" spans="2:11" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="B74" s="8" t="s">
+      <c r="B74" s="12" t="s">
         <v>11</v>
       </c>
       <c r="C74" s="21"/>
@@ -2734,7 +2734,7 @@
       <c r="K75" s="20"/>
     </row>
     <row r="76" spans="2:11" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="B76" s="8" t="s">
+      <c r="B76" s="12" t="s">
         <v>10</v>
       </c>
       <c r="C76" s="21"/>
@@ -2844,36 +2844,36 @@
       <c r="K83" s="20"/>
     </row>
     <row r="84" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B84" s="4" t="s">
+      <c r="B84" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="C84" s="5"/>
-      <c r="D84" s="5" t="s">
+      <c r="C84" s="9"/>
+      <c r="D84" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="E84" s="5"/>
-      <c r="F84" s="5"/>
-      <c r="G84" s="5"/>
-      <c r="H84" s="5"/>
-      <c r="I84" s="5"/>
-      <c r="J84" s="6" t="s">
+      <c r="E84" s="9"/>
+      <c r="F84" s="9"/>
+      <c r="G84" s="9"/>
+      <c r="H84" s="9"/>
+      <c r="I84" s="9"/>
+      <c r="J84" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="K84" s="7"/>
+      <c r="K84" s="11"/>
     </row>
     <row r="85" spans="2:11" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="B85" s="8" t="s">
+      <c r="B85" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C85" s="9"/>
-      <c r="D85" s="9"/>
-      <c r="E85" s="9"/>
-      <c r="F85" s="9"/>
-      <c r="G85" s="9"/>
-      <c r="H85" s="9"/>
-      <c r="I85" s="9"/>
-      <c r="J85" s="9"/>
-      <c r="K85" s="10"/>
+      <c r="C85" s="13"/>
+      <c r="D85" s="13"/>
+      <c r="E85" s="13"/>
+      <c r="F85" s="13"/>
+      <c r="G85" s="13"/>
+      <c r="H85" s="13"/>
+      <c r="I85" s="13"/>
+      <c r="J85" s="13"/>
+      <c r="K85" s="14"/>
     </row>
     <row r="86" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B86" s="18" t="s">
@@ -2896,112 +2896,112 @@
       <c r="K86" s="20"/>
     </row>
     <row r="87" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B87" s="4" t="s">
+      <c r="B87" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="C87" s="5"/>
-      <c r="D87" s="5" t="s">
+      <c r="C87" s="9"/>
+      <c r="D87" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="E87" s="5"/>
-      <c r="F87" s="5" t="s">
+      <c r="E87" s="9"/>
+      <c r="F87" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="G87" s="5"/>
-      <c r="H87" s="5"/>
-      <c r="I87" s="5"/>
-      <c r="J87" s="6" t="s">
+      <c r="G87" s="9"/>
+      <c r="H87" s="9"/>
+      <c r="I87" s="9"/>
+      <c r="J87" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="K87" s="7"/>
+      <c r="K87" s="11"/>
     </row>
     <row r="88" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B88" s="4" t="s">
+      <c r="B88" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="C88" s="5"/>
-      <c r="D88" s="5" t="s">
+      <c r="C88" s="9"/>
+      <c r="D88" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="E88" s="5"/>
-      <c r="F88" s="5" t="s">
+      <c r="E88" s="9"/>
+      <c r="F88" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="G88" s="5"/>
-      <c r="H88" s="5"/>
-      <c r="I88" s="5"/>
-      <c r="J88" s="6" t="s">
+      <c r="G88" s="9"/>
+      <c r="H88" s="9"/>
+      <c r="I88" s="9"/>
+      <c r="J88" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="K88" s="7"/>
+      <c r="K88" s="11"/>
     </row>
     <row r="89" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B89" s="4" t="s">
+      <c r="B89" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C89" s="5"/>
-      <c r="D89" s="5" t="s">
+      <c r="C89" s="9"/>
+      <c r="D89" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="E89" s="5"/>
-      <c r="F89" s="5" t="s">
+      <c r="E89" s="9"/>
+      <c r="F89" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="G89" s="5"/>
-      <c r="H89" s="5"/>
-      <c r="I89" s="5"/>
-      <c r="J89" s="6" t="s">
+      <c r="G89" s="9"/>
+      <c r="H89" s="9"/>
+      <c r="I89" s="9"/>
+      <c r="J89" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="K89" s="7"/>
+      <c r="K89" s="11"/>
     </row>
     <row r="90" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B90" s="4" t="s">
+      <c r="B90" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="C90" s="5"/>
-      <c r="D90" s="5" t="s">
+      <c r="C90" s="9"/>
+      <c r="D90" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="E90" s="5"/>
-      <c r="F90" s="5" t="s">
+      <c r="E90" s="9"/>
+      <c r="F90" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="G90" s="5"/>
-      <c r="H90" s="5"/>
-      <c r="I90" s="5"/>
-      <c r="J90" s="6" t="s">
+      <c r="G90" s="9"/>
+      <c r="H90" s="9"/>
+      <c r="I90" s="9"/>
+      <c r="J90" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="K90" s="7"/>
+      <c r="K90" s="11"/>
     </row>
     <row r="91" spans="2:11" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="B91" s="8" t="s">
+      <c r="B91" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="C91" s="9"/>
-      <c r="D91" s="9"/>
-      <c r="E91" s="9"/>
-      <c r="F91" s="9"/>
-      <c r="G91" s="9"/>
-      <c r="H91" s="9"/>
-      <c r="I91" s="9"/>
-      <c r="J91" s="9"/>
-      <c r="K91" s="10"/>
+      <c r="C91" s="13"/>
+      <c r="D91" s="13"/>
+      <c r="E91" s="13"/>
+      <c r="F91" s="13"/>
+      <c r="G91" s="13"/>
+      <c r="H91" s="13"/>
+      <c r="I91" s="13"/>
+      <c r="J91" s="13"/>
+      <c r="K91" s="14"/>
     </row>
     <row r="92" spans="2:11" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B92" s="11" t="s">
+      <c r="B92" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="C92" s="12"/>
-      <c r="D92" s="12"/>
-      <c r="E92" s="12"/>
-      <c r="F92" s="12"/>
-      <c r="G92" s="12"/>
-      <c r="H92" s="12"/>
-      <c r="I92" s="12"/>
-      <c r="J92" s="12"/>
-      <c r="K92" s="13"/>
+      <c r="C92" s="16"/>
+      <c r="D92" s="16"/>
+      <c r="E92" s="16"/>
+      <c r="F92" s="16"/>
+      <c r="G92" s="16"/>
+      <c r="H92" s="16"/>
+      <c r="I92" s="16"/>
+      <c r="J92" s="16"/>
+      <c r="K92" s="17"/>
     </row>
     <row r="93" spans="2:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="94" spans="2:11" ht="41.25" x14ac:dyDescent="0.3">
@@ -3149,7 +3149,7 @@
       <c r="K103" s="40"/>
     </row>
     <row r="104" spans="2:11" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="B104" s="8" t="s">
+      <c r="B104" s="12" t="s">
         <v>11</v>
       </c>
       <c r="C104" s="21"/>
@@ -3183,27 +3183,27 @@
       <c r="K105" s="20"/>
     </row>
     <row r="106" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B106" s="14" t="s">
+      <c r="B106" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C106" s="15"/>
-      <c r="D106" s="15" t="s">
+      <c r="C106" s="5"/>
+      <c r="D106" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E106" s="15"/>
-      <c r="F106" s="15" t="s">
+      <c r="E106" s="5"/>
+      <c r="F106" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="G106" s="15"/>
-      <c r="H106" s="15"/>
-      <c r="I106" s="15"/>
-      <c r="J106" s="15" t="s">
+      <c r="G106" s="5"/>
+      <c r="H106" s="5"/>
+      <c r="I106" s="5"/>
+      <c r="J106" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="K106" s="17"/>
+      <c r="K106" s="7"/>
     </row>
     <row r="107" spans="2:11" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="B107" s="8" t="s">
+      <c r="B107" s="12" t="s">
         <v>10</v>
       </c>
       <c r="C107" s="21"/>
@@ -3313,36 +3313,36 @@
       <c r="K114" s="20"/>
     </row>
     <row r="115" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B115" s="4" t="s">
+      <c r="B115" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="C115" s="5"/>
-      <c r="D115" s="5" t="s">
+      <c r="C115" s="9"/>
+      <c r="D115" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="E115" s="5"/>
-      <c r="F115" s="5"/>
-      <c r="G115" s="5"/>
-      <c r="H115" s="5"/>
-      <c r="I115" s="5"/>
-      <c r="J115" s="6" t="s">
+      <c r="E115" s="9"/>
+      <c r="F115" s="9"/>
+      <c r="G115" s="9"/>
+      <c r="H115" s="9"/>
+      <c r="I115" s="9"/>
+      <c r="J115" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="K115" s="7"/>
+      <c r="K115" s="11"/>
     </row>
     <row r="116" spans="2:11" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="B116" s="8" t="s">
+      <c r="B116" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C116" s="9"/>
-      <c r="D116" s="9"/>
-      <c r="E116" s="9"/>
-      <c r="F116" s="9"/>
-      <c r="G116" s="9"/>
-      <c r="H116" s="9"/>
-      <c r="I116" s="9"/>
-      <c r="J116" s="9"/>
-      <c r="K116" s="10"/>
+      <c r="C116" s="13"/>
+      <c r="D116" s="13"/>
+      <c r="E116" s="13"/>
+      <c r="F116" s="13"/>
+      <c r="G116" s="13"/>
+      <c r="H116" s="13"/>
+      <c r="I116" s="13"/>
+      <c r="J116" s="13"/>
+      <c r="K116" s="14"/>
     </row>
     <row r="117" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B117" s="18" t="s">
@@ -3365,72 +3365,72 @@
       <c r="K117" s="20"/>
     </row>
     <row r="118" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B118" s="4" t="s">
+      <c r="B118" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="C118" s="5"/>
-      <c r="D118" s="5" t="s">
+      <c r="C118" s="9"/>
+      <c r="D118" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="E118" s="5"/>
-      <c r="F118" s="5" t="s">
+      <c r="E118" s="9"/>
+      <c r="F118" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="G118" s="5"/>
-      <c r="H118" s="5"/>
-      <c r="I118" s="5"/>
-      <c r="J118" s="6" t="s">
+      <c r="G118" s="9"/>
+      <c r="H118" s="9"/>
+      <c r="I118" s="9"/>
+      <c r="J118" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="K118" s="7"/>
+      <c r="K118" s="11"/>
     </row>
     <row r="119" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B119" s="4" t="s">
+      <c r="B119" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="C119" s="5"/>
-      <c r="D119" s="5" t="s">
+      <c r="C119" s="9"/>
+      <c r="D119" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="E119" s="5"/>
-      <c r="F119" s="5" t="s">
+      <c r="E119" s="9"/>
+      <c r="F119" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="G119" s="5"/>
-      <c r="H119" s="5"/>
-      <c r="I119" s="5"/>
-      <c r="J119" s="6" t="s">
+      <c r="G119" s="9"/>
+      <c r="H119" s="9"/>
+      <c r="I119" s="9"/>
+      <c r="J119" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="K119" s="7"/>
+      <c r="K119" s="11"/>
     </row>
     <row r="120" spans="2:11" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="B120" s="8" t="s">
+      <c r="B120" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="C120" s="9"/>
-      <c r="D120" s="9"/>
-      <c r="E120" s="9"/>
-      <c r="F120" s="9"/>
-      <c r="G120" s="9"/>
-      <c r="H120" s="9"/>
-      <c r="I120" s="9"/>
-      <c r="J120" s="9"/>
-      <c r="K120" s="10"/>
+      <c r="C120" s="13"/>
+      <c r="D120" s="13"/>
+      <c r="E120" s="13"/>
+      <c r="F120" s="13"/>
+      <c r="G120" s="13"/>
+      <c r="H120" s="13"/>
+      <c r="I120" s="13"/>
+      <c r="J120" s="13"/>
+      <c r="K120" s="14"/>
     </row>
     <row r="121" spans="2:11" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B121" s="11" t="s">
+      <c r="B121" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="C121" s="12"/>
-      <c r="D121" s="12"/>
-      <c r="E121" s="12"/>
-      <c r="F121" s="12"/>
-      <c r="G121" s="12"/>
-      <c r="H121" s="12"/>
-      <c r="I121" s="12"/>
-      <c r="J121" s="12"/>
-      <c r="K121" s="13"/>
+      <c r="C121" s="16"/>
+      <c r="D121" s="16"/>
+      <c r="E121" s="16"/>
+      <c r="F121" s="16"/>
+      <c r="G121" s="16"/>
+      <c r="H121" s="16"/>
+      <c r="I121" s="16"/>
+      <c r="J121" s="16"/>
+      <c r="K121" s="17"/>
     </row>
     <row r="122" spans="2:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="123" spans="2:11" ht="41.25" x14ac:dyDescent="0.3">
@@ -3578,7 +3578,7 @@
       <c r="K132" s="40"/>
     </row>
     <row r="133" spans="2:11" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="B133" s="8" t="s">
+      <c r="B133" s="12" t="s">
         <v>11</v>
       </c>
       <c r="C133" s="21"/>
@@ -3612,27 +3612,27 @@
       <c r="K134" s="20"/>
     </row>
     <row r="135" spans="2:11" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B135" s="14" t="s">
+      <c r="B135" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="C135" s="15"/>
-      <c r="D135" s="15" t="s">
+      <c r="C135" s="5"/>
+      <c r="D135" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E135" s="15"/>
-      <c r="F135" s="16" t="s">
+      <c r="E135" s="5"/>
+      <c r="F135" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="G135" s="15"/>
-      <c r="H135" s="15"/>
-      <c r="I135" s="15"/>
-      <c r="J135" s="15" t="s">
+      <c r="G135" s="5"/>
+      <c r="H135" s="5"/>
+      <c r="I135" s="5"/>
+      <c r="J135" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="K135" s="17"/>
+      <c r="K135" s="7"/>
     </row>
     <row r="136" spans="2:11" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="B136" s="8" t="s">
+      <c r="B136" s="12" t="s">
         <v>10</v>
       </c>
       <c r="C136" s="21"/>
@@ -3742,36 +3742,36 @@
       <c r="K143" s="20"/>
     </row>
     <row r="144" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B144" s="4" t="s">
+      <c r="B144" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="C144" s="5"/>
-      <c r="D144" s="5" t="s">
+      <c r="C144" s="9"/>
+      <c r="D144" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="E144" s="5"/>
-      <c r="F144" s="5"/>
-      <c r="G144" s="5"/>
-      <c r="H144" s="5"/>
-      <c r="I144" s="5"/>
-      <c r="J144" s="6" t="s">
+      <c r="E144" s="9"/>
+      <c r="F144" s="9"/>
+      <c r="G144" s="9"/>
+      <c r="H144" s="9"/>
+      <c r="I144" s="9"/>
+      <c r="J144" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="K144" s="7"/>
+      <c r="K144" s="11"/>
     </row>
     <row r="145" spans="2:11" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="B145" s="8" t="s">
+      <c r="B145" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C145" s="9"/>
-      <c r="D145" s="9"/>
-      <c r="E145" s="9"/>
-      <c r="F145" s="9"/>
-      <c r="G145" s="9"/>
-      <c r="H145" s="9"/>
-      <c r="I145" s="9"/>
-      <c r="J145" s="9"/>
-      <c r="K145" s="10"/>
+      <c r="C145" s="13"/>
+      <c r="D145" s="13"/>
+      <c r="E145" s="13"/>
+      <c r="F145" s="13"/>
+      <c r="G145" s="13"/>
+      <c r="H145" s="13"/>
+      <c r="I145" s="13"/>
+      <c r="J145" s="13"/>
+      <c r="K145" s="14"/>
     </row>
     <row r="146" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B146" s="18" t="s">
@@ -3794,72 +3794,72 @@
       <c r="K146" s="20"/>
     </row>
     <row r="147" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B147" s="4" t="s">
+      <c r="B147" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="C147" s="5"/>
-      <c r="D147" s="5" t="s">
+      <c r="C147" s="9"/>
+      <c r="D147" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="E147" s="5"/>
-      <c r="F147" s="5" t="s">
+      <c r="E147" s="9"/>
+      <c r="F147" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="G147" s="5"/>
-      <c r="H147" s="5"/>
-      <c r="I147" s="5"/>
-      <c r="J147" s="6" t="s">
+      <c r="G147" s="9"/>
+      <c r="H147" s="9"/>
+      <c r="I147" s="9"/>
+      <c r="J147" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="K147" s="7"/>
+      <c r="K147" s="11"/>
     </row>
     <row r="148" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B148" s="4" t="s">
+      <c r="B148" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="C148" s="5"/>
-      <c r="D148" s="5" t="s">
+      <c r="C148" s="9"/>
+      <c r="D148" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="E148" s="5"/>
-      <c r="F148" s="5" t="s">
+      <c r="E148" s="9"/>
+      <c r="F148" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="G148" s="5"/>
-      <c r="H148" s="5"/>
-      <c r="I148" s="5"/>
-      <c r="J148" s="6" t="s">
+      <c r="G148" s="9"/>
+      <c r="H148" s="9"/>
+      <c r="I148" s="9"/>
+      <c r="J148" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="K148" s="7"/>
+      <c r="K148" s="11"/>
     </row>
     <row r="149" spans="2:11" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="B149" s="8" t="s">
+      <c r="B149" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="C149" s="9"/>
-      <c r="D149" s="9"/>
-      <c r="E149" s="9"/>
-      <c r="F149" s="9"/>
-      <c r="G149" s="9"/>
-      <c r="H149" s="9"/>
-      <c r="I149" s="9"/>
-      <c r="J149" s="9"/>
-      <c r="K149" s="10"/>
+      <c r="C149" s="13"/>
+      <c r="D149" s="13"/>
+      <c r="E149" s="13"/>
+      <c r="F149" s="13"/>
+      <c r="G149" s="13"/>
+      <c r="H149" s="13"/>
+      <c r="I149" s="13"/>
+      <c r="J149" s="13"/>
+      <c r="K149" s="14"/>
     </row>
     <row r="150" spans="2:11" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B150" s="11" t="s">
+      <c r="B150" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="C150" s="12"/>
-      <c r="D150" s="12"/>
-      <c r="E150" s="12"/>
-      <c r="F150" s="12"/>
-      <c r="G150" s="12"/>
-      <c r="H150" s="12"/>
-      <c r="I150" s="12"/>
-      <c r="J150" s="12"/>
-      <c r="K150" s="13"/>
+      <c r="C150" s="16"/>
+      <c r="D150" s="16"/>
+      <c r="E150" s="16"/>
+      <c r="F150" s="16"/>
+      <c r="G150" s="16"/>
+      <c r="H150" s="16"/>
+      <c r="I150" s="16"/>
+      <c r="J150" s="16"/>
+      <c r="K150" s="17"/>
     </row>
     <row r="151" spans="2:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="152" spans="2:11" ht="41.25" x14ac:dyDescent="0.3">
@@ -4007,7 +4007,7 @@
       <c r="K161" s="40"/>
     </row>
     <row r="162" spans="2:11" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="B162" s="8" t="s">
+      <c r="B162" s="12" t="s">
         <v>11</v>
       </c>
       <c r="C162" s="21"/>
@@ -4041,47 +4041,47 @@
       <c r="K163" s="20"/>
     </row>
     <row r="164" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B164" s="14" t="s">
+      <c r="B164" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="C164" s="15"/>
-      <c r="D164" s="15" t="s">
+      <c r="C164" s="5"/>
+      <c r="D164" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E164" s="15"/>
-      <c r="F164" s="16" t="s">
+      <c r="E164" s="5"/>
+      <c r="F164" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="G164" s="15"/>
-      <c r="H164" s="15"/>
-      <c r="I164" s="15"/>
-      <c r="J164" s="15" t="s">
+      <c r="G164" s="5"/>
+      <c r="H164" s="5"/>
+      <c r="I164" s="5"/>
+      <c r="J164" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="K164" s="17"/>
+      <c r="K164" s="7"/>
     </row>
     <row r="165" spans="2:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B165" s="14" t="s">
+      <c r="B165" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="C165" s="15"/>
-      <c r="D165" s="15" t="s">
+      <c r="C165" s="5"/>
+      <c r="D165" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E165" s="15"/>
-      <c r="F165" s="16" t="s">
+      <c r="E165" s="5"/>
+      <c r="F165" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="G165" s="15"/>
-      <c r="H165" s="15"/>
-      <c r="I165" s="15"/>
-      <c r="J165" s="15" t="s">
+      <c r="G165" s="5"/>
+      <c r="H165" s="5"/>
+      <c r="I165" s="5"/>
+      <c r="J165" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="K165" s="17"/>
+      <c r="K165" s="7"/>
     </row>
     <row r="166" spans="2:11" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="B166" s="8" t="s">
+      <c r="B166" s="12" t="s">
         <v>10</v>
       </c>
       <c r="C166" s="21"/>
@@ -4191,36 +4191,36 @@
       <c r="K173" s="20"/>
     </row>
     <row r="174" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B174" s="4" t="s">
+      <c r="B174" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="C174" s="5"/>
-      <c r="D174" s="5" t="s">
+      <c r="C174" s="9"/>
+      <c r="D174" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="E174" s="5"/>
-      <c r="F174" s="5"/>
-      <c r="G174" s="5"/>
-      <c r="H174" s="5"/>
-      <c r="I174" s="5"/>
-      <c r="J174" s="6" t="s">
+      <c r="E174" s="9"/>
+      <c r="F174" s="9"/>
+      <c r="G174" s="9"/>
+      <c r="H174" s="9"/>
+      <c r="I174" s="9"/>
+      <c r="J174" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="K174" s="7"/>
+      <c r="K174" s="11"/>
     </row>
     <row r="175" spans="2:11" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="B175" s="8" t="s">
+      <c r="B175" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C175" s="9"/>
-      <c r="D175" s="9"/>
-      <c r="E175" s="9"/>
-      <c r="F175" s="9"/>
-      <c r="G175" s="9"/>
-      <c r="H175" s="9"/>
-      <c r="I175" s="9"/>
-      <c r="J175" s="9"/>
-      <c r="K175" s="10"/>
+      <c r="C175" s="13"/>
+      <c r="D175" s="13"/>
+      <c r="E175" s="13"/>
+      <c r="F175" s="13"/>
+      <c r="G175" s="13"/>
+      <c r="H175" s="13"/>
+      <c r="I175" s="13"/>
+      <c r="J175" s="13"/>
+      <c r="K175" s="14"/>
     </row>
     <row r="176" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B176" s="18" t="s">
@@ -4243,72 +4243,72 @@
       <c r="K176" s="20"/>
     </row>
     <row r="177" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B177" s="4" t="s">
+      <c r="B177" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="C177" s="5"/>
-      <c r="D177" s="5" t="s">
+      <c r="C177" s="9"/>
+      <c r="D177" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="E177" s="5"/>
-      <c r="F177" s="5" t="s">
+      <c r="E177" s="9"/>
+      <c r="F177" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="G177" s="5"/>
-      <c r="H177" s="5"/>
-      <c r="I177" s="5"/>
-      <c r="J177" s="6" t="s">
+      <c r="G177" s="9"/>
+      <c r="H177" s="9"/>
+      <c r="I177" s="9"/>
+      <c r="J177" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="K177" s="7"/>
+      <c r="K177" s="11"/>
     </row>
     <row r="178" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B178" s="4" t="s">
+      <c r="B178" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="C178" s="5"/>
-      <c r="D178" s="5" t="s">
+      <c r="C178" s="9"/>
+      <c r="D178" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="E178" s="5"/>
-      <c r="F178" s="5" t="s">
+      <c r="E178" s="9"/>
+      <c r="F178" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="G178" s="5"/>
-      <c r="H178" s="5"/>
-      <c r="I178" s="5"/>
-      <c r="J178" s="6" t="s">
+      <c r="G178" s="9"/>
+      <c r="H178" s="9"/>
+      <c r="I178" s="9"/>
+      <c r="J178" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="K178" s="7"/>
+      <c r="K178" s="11"/>
     </row>
     <row r="179" spans="2:11" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="B179" s="8" t="s">
+      <c r="B179" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="C179" s="9"/>
-      <c r="D179" s="9"/>
-      <c r="E179" s="9"/>
-      <c r="F179" s="9"/>
-      <c r="G179" s="9"/>
-      <c r="H179" s="9"/>
-      <c r="I179" s="9"/>
-      <c r="J179" s="9"/>
-      <c r="K179" s="10"/>
+      <c r="C179" s="13"/>
+      <c r="D179" s="13"/>
+      <c r="E179" s="13"/>
+      <c r="F179" s="13"/>
+      <c r="G179" s="13"/>
+      <c r="H179" s="13"/>
+      <c r="I179" s="13"/>
+      <c r="J179" s="13"/>
+      <c r="K179" s="14"/>
     </row>
     <row r="180" spans="2:11" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B180" s="11" t="s">
+      <c r="B180" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="C180" s="12"/>
-      <c r="D180" s="12"/>
-      <c r="E180" s="12"/>
-      <c r="F180" s="12"/>
-      <c r="G180" s="12"/>
-      <c r="H180" s="12"/>
-      <c r="I180" s="12"/>
-      <c r="J180" s="12"/>
-      <c r="K180" s="13"/>
+      <c r="C180" s="16"/>
+      <c r="D180" s="16"/>
+      <c r="E180" s="16"/>
+      <c r="F180" s="16"/>
+      <c r="G180" s="16"/>
+      <c r="H180" s="16"/>
+      <c r="I180" s="16"/>
+      <c r="J180" s="16"/>
+      <c r="K180" s="17"/>
     </row>
     <row r="181" spans="2:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="182" spans="2:11" ht="41.25" x14ac:dyDescent="0.3">
@@ -4456,7 +4456,7 @@
       <c r="K191" s="40"/>
     </row>
     <row r="192" spans="2:11" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="B192" s="8" t="s">
+      <c r="B192" s="12" t="s">
         <v>11</v>
       </c>
       <c r="C192" s="21"/>
@@ -4490,90 +4490,90 @@
       <c r="K193" s="20"/>
     </row>
     <row r="194" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B194" s="14" t="s">
+      <c r="B194" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C194" s="15"/>
-      <c r="D194" s="15" t="s">
+      <c r="C194" s="5"/>
+      <c r="D194" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E194" s="15"/>
-      <c r="F194" s="16" t="s">
+      <c r="E194" s="5"/>
+      <c r="F194" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="G194" s="15"/>
-      <c r="H194" s="15"/>
-      <c r="I194" s="15"/>
-      <c r="J194" s="15" t="s">
+      <c r="G194" s="5"/>
+      <c r="H194" s="5"/>
+      <c r="I194" s="5"/>
+      <c r="J194" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="K194" s="17"/>
+      <c r="K194" s="7"/>
     </row>
     <row r="195" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B195" s="14" t="s">
+      <c r="B195" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C195" s="15"/>
-      <c r="D195" s="15" t="s">
+      <c r="C195" s="5"/>
+      <c r="D195" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E195" s="15"/>
-      <c r="F195" s="16" t="s">
+      <c r="E195" s="5"/>
+      <c r="F195" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="G195" s="15"/>
-      <c r="H195" s="15"/>
-      <c r="I195" s="15"/>
-      <c r="J195" s="15" t="s">
+      <c r="G195" s="5"/>
+      <c r="H195" s="5"/>
+      <c r="I195" s="5"/>
+      <c r="J195" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="K195" s="17"/>
+      <c r="K195" s="7"/>
     </row>
     <row r="196" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B196" s="14" t="s">
+      <c r="B196" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="C196" s="15"/>
-      <c r="D196" s="15" t="s">
+      <c r="C196" s="5"/>
+      <c r="D196" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E196" s="15"/>
-      <c r="F196" s="16" t="s">
+      <c r="E196" s="5"/>
+      <c r="F196" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="G196" s="15"/>
-      <c r="H196" s="15"/>
-      <c r="I196" s="15"/>
-      <c r="J196" s="15" t="s">
+      <c r="G196" s="5"/>
+      <c r="H196" s="5"/>
+      <c r="I196" s="5"/>
+      <c r="J196" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="K196" s="17"/>
+      <c r="K196" s="7"/>
     </row>
     <row r="197" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
         <v>71</v>
       </c>
-      <c r="B197" s="14" t="s">
+      <c r="B197" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="C197" s="15"/>
-      <c r="D197" s="15" t="s">
+      <c r="C197" s="5"/>
+      <c r="D197" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E197" s="15"/>
-      <c r="F197" s="16" t="s">
+      <c r="E197" s="5"/>
+      <c r="F197" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="G197" s="15"/>
-      <c r="H197" s="15"/>
-      <c r="I197" s="15"/>
-      <c r="J197" s="15" t="s">
+      <c r="G197" s="5"/>
+      <c r="H197" s="5"/>
+      <c r="I197" s="5"/>
+      <c r="J197" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="K197" s="17"/>
+      <c r="K197" s="7"/>
     </row>
     <row r="198" spans="1:11" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="B198" s="8" t="s">
+      <c r="B198" s="12" t="s">
         <v>10</v>
       </c>
       <c r="C198" s="21"/>
@@ -4683,36 +4683,36 @@
       <c r="K205" s="20"/>
     </row>
     <row r="206" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B206" s="4" t="s">
+      <c r="B206" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="C206" s="5"/>
-      <c r="D206" s="5" t="s">
+      <c r="C206" s="9"/>
+      <c r="D206" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="E206" s="5"/>
-      <c r="F206" s="5"/>
-      <c r="G206" s="5"/>
-      <c r="H206" s="5"/>
-      <c r="I206" s="5"/>
-      <c r="J206" s="6" t="s">
+      <c r="E206" s="9"/>
+      <c r="F206" s="9"/>
+      <c r="G206" s="9"/>
+      <c r="H206" s="9"/>
+      <c r="I206" s="9"/>
+      <c r="J206" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="K206" s="7"/>
+      <c r="K206" s="11"/>
     </row>
     <row r="207" spans="1:11" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="B207" s="8" t="s">
+      <c r="B207" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C207" s="9"/>
-      <c r="D207" s="9"/>
-      <c r="E207" s="9"/>
-      <c r="F207" s="9"/>
-      <c r="G207" s="9"/>
-      <c r="H207" s="9"/>
-      <c r="I207" s="9"/>
-      <c r="J207" s="9"/>
-      <c r="K207" s="10"/>
+      <c r="C207" s="13"/>
+      <c r="D207" s="13"/>
+      <c r="E207" s="13"/>
+      <c r="F207" s="13"/>
+      <c r="G207" s="13"/>
+      <c r="H207" s="13"/>
+      <c r="I207" s="13"/>
+      <c r="J207" s="13"/>
+      <c r="K207" s="14"/>
     </row>
     <row r="208" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B208" s="18" t="s">
@@ -4735,84 +4735,354 @@
       <c r="K208" s="20"/>
     </row>
     <row r="209" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B209" s="4" t="s">
+      <c r="B209" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="C209" s="5"/>
-      <c r="D209" s="5" t="s">
+      <c r="C209" s="9"/>
+      <c r="D209" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="E209" s="5"/>
-      <c r="F209" s="5" t="s">
+      <c r="E209" s="9"/>
+      <c r="F209" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="G209" s="5"/>
-      <c r="H209" s="5"/>
-      <c r="I209" s="5"/>
-      <c r="J209" s="6" t="s">
+      <c r="G209" s="9"/>
+      <c r="H209" s="9"/>
+      <c r="I209" s="9"/>
+      <c r="J209" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="K209" s="7"/>
+      <c r="K209" s="11"/>
     </row>
     <row r="210" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B210" s="4" t="s">
+      <c r="B210" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="C210" s="5"/>
-      <c r="D210" s="5" t="s">
+      <c r="C210" s="9"/>
+      <c r="D210" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="E210" s="5"/>
-      <c r="F210" s="5" t="s">
+      <c r="E210" s="9"/>
+      <c r="F210" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="G210" s="5"/>
-      <c r="H210" s="5"/>
-      <c r="I210" s="5"/>
-      <c r="J210" s="6" t="s">
+      <c r="G210" s="9"/>
+      <c r="H210" s="9"/>
+      <c r="I210" s="9"/>
+      <c r="J210" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="K210" s="7"/>
+      <c r="K210" s="11"/>
     </row>
     <row r="211" spans="2:11" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="B211" s="8" t="s">
+      <c r="B211" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="C211" s="9"/>
-      <c r="D211" s="9"/>
-      <c r="E211" s="9"/>
-      <c r="F211" s="9"/>
-      <c r="G211" s="9"/>
-      <c r="H211" s="9"/>
-      <c r="I211" s="9"/>
-      <c r="J211" s="9"/>
-      <c r="K211" s="10"/>
+      <c r="C211" s="13"/>
+      <c r="D211" s="13"/>
+      <c r="E211" s="13"/>
+      <c r="F211" s="13"/>
+      <c r="G211" s="13"/>
+      <c r="H211" s="13"/>
+      <c r="I211" s="13"/>
+      <c r="J211" s="13"/>
+      <c r="K211" s="14"/>
     </row>
     <row r="212" spans="2:11" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B212" s="11" t="s">
+      <c r="B212" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="C212" s="12"/>
-      <c r="D212" s="12"/>
-      <c r="E212" s="12"/>
-      <c r="F212" s="12"/>
-      <c r="G212" s="12"/>
-      <c r="H212" s="12"/>
-      <c r="I212" s="12"/>
-      <c r="J212" s="12"/>
-      <c r="K212" s="13"/>
+      <c r="C212" s="16"/>
+      <c r="D212" s="16"/>
+      <c r="E212" s="16"/>
+      <c r="F212" s="16"/>
+      <c r="G212" s="16"/>
+      <c r="H212" s="16"/>
+      <c r="I212" s="16"/>
+      <c r="J212" s="16"/>
+      <c r="K212" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="316">
-    <mergeCell ref="B195:C195"/>
-    <mergeCell ref="D195:E195"/>
-    <mergeCell ref="F195:I195"/>
-    <mergeCell ref="J195:K195"/>
-    <mergeCell ref="B210:C210"/>
-    <mergeCell ref="D210:E210"/>
-    <mergeCell ref="F210:I210"/>
-    <mergeCell ref="J210:K210"/>
-    <mergeCell ref="B211:K211"/>
+    <mergeCell ref="B178:C178"/>
+    <mergeCell ref="D178:E178"/>
+    <mergeCell ref="F178:I178"/>
+    <mergeCell ref="J178:K178"/>
+    <mergeCell ref="B179:K179"/>
+    <mergeCell ref="B180:K180"/>
+    <mergeCell ref="B165:C165"/>
+    <mergeCell ref="D165:E165"/>
+    <mergeCell ref="F165:I165"/>
+    <mergeCell ref="J165:K165"/>
+    <mergeCell ref="B175:K175"/>
+    <mergeCell ref="B176:C176"/>
+    <mergeCell ref="D176:E176"/>
+    <mergeCell ref="F176:I176"/>
+    <mergeCell ref="J176:K176"/>
+    <mergeCell ref="B177:C177"/>
+    <mergeCell ref="D177:E177"/>
+    <mergeCell ref="F177:I177"/>
+    <mergeCell ref="J177:K177"/>
+    <mergeCell ref="B166:K166"/>
+    <mergeCell ref="B167:K170"/>
+    <mergeCell ref="B171:K171"/>
+    <mergeCell ref="B172:K172"/>
+    <mergeCell ref="B173:C173"/>
+    <mergeCell ref="D173:I173"/>
+    <mergeCell ref="J173:K173"/>
+    <mergeCell ref="B174:C174"/>
+    <mergeCell ref="D174:I174"/>
+    <mergeCell ref="J174:K174"/>
+    <mergeCell ref="B161:C161"/>
+    <mergeCell ref="D161:I161"/>
+    <mergeCell ref="J161:K161"/>
+    <mergeCell ref="B162:K162"/>
+    <mergeCell ref="B163:C163"/>
+    <mergeCell ref="D163:E163"/>
+    <mergeCell ref="F163:I163"/>
+    <mergeCell ref="J163:K163"/>
+    <mergeCell ref="B164:C164"/>
+    <mergeCell ref="D164:E164"/>
+    <mergeCell ref="F164:I164"/>
+    <mergeCell ref="J164:K164"/>
+    <mergeCell ref="B152:K152"/>
+    <mergeCell ref="B153:K153"/>
+    <mergeCell ref="B154:K157"/>
+    <mergeCell ref="B158:C158"/>
+    <mergeCell ref="D158:F158"/>
+    <mergeCell ref="G158:H158"/>
+    <mergeCell ref="I158:K158"/>
+    <mergeCell ref="B159:K159"/>
+    <mergeCell ref="B160:K160"/>
+    <mergeCell ref="B91:K91"/>
+    <mergeCell ref="B92:K92"/>
+    <mergeCell ref="B89:C89"/>
+    <mergeCell ref="D89:E89"/>
+    <mergeCell ref="F89:I89"/>
+    <mergeCell ref="J89:K89"/>
+    <mergeCell ref="B90:C90"/>
+    <mergeCell ref="D90:E90"/>
+    <mergeCell ref="F90:I90"/>
+    <mergeCell ref="J90:K90"/>
+    <mergeCell ref="B88:C88"/>
+    <mergeCell ref="D88:E88"/>
+    <mergeCell ref="F88:I88"/>
+    <mergeCell ref="J88:K88"/>
+    <mergeCell ref="B84:C84"/>
+    <mergeCell ref="D84:I84"/>
+    <mergeCell ref="J84:K84"/>
+    <mergeCell ref="B85:K85"/>
+    <mergeCell ref="B86:C86"/>
+    <mergeCell ref="D86:E86"/>
+    <mergeCell ref="F86:I86"/>
+    <mergeCell ref="J86:K86"/>
+    <mergeCell ref="B76:K76"/>
+    <mergeCell ref="B77:K80"/>
+    <mergeCell ref="B81:K81"/>
+    <mergeCell ref="B82:K82"/>
+    <mergeCell ref="B83:C83"/>
+    <mergeCell ref="D83:I83"/>
+    <mergeCell ref="J83:K83"/>
+    <mergeCell ref="B87:C87"/>
+    <mergeCell ref="D87:E87"/>
+    <mergeCell ref="F87:I87"/>
+    <mergeCell ref="J87:K87"/>
+    <mergeCell ref="B31:K31"/>
+    <mergeCell ref="B32:K32"/>
+    <mergeCell ref="B74:K74"/>
+    <mergeCell ref="B75:C75"/>
+    <mergeCell ref="D75:E75"/>
+    <mergeCell ref="F75:I75"/>
+    <mergeCell ref="J75:K75"/>
+    <mergeCell ref="B71:K71"/>
+    <mergeCell ref="B72:K72"/>
+    <mergeCell ref="B73:C73"/>
+    <mergeCell ref="D73:I73"/>
+    <mergeCell ref="J73:K73"/>
+    <mergeCell ref="B51:K51"/>
+    <mergeCell ref="J40:K40"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="J41:K41"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="D53:I53"/>
+    <mergeCell ref="J53:K53"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="F44:I44"/>
+    <mergeCell ref="J44:K44"/>
+    <mergeCell ref="B64:K64"/>
+    <mergeCell ref="B65:K65"/>
+    <mergeCell ref="B66:K69"/>
+    <mergeCell ref="B70:C70"/>
+    <mergeCell ref="D70:F70"/>
+    <mergeCell ref="G70:H70"/>
+    <mergeCell ref="I70:K70"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="D57:E57"/>
+    <mergeCell ref="F57:I57"/>
+    <mergeCell ref="J57:K57"/>
+    <mergeCell ref="B62:K62"/>
+    <mergeCell ref="F59:I59"/>
+    <mergeCell ref="J59:K59"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="D58:E58"/>
+    <mergeCell ref="F58:I58"/>
+    <mergeCell ref="J58:K58"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="D54:I54"/>
+    <mergeCell ref="J54:K54"/>
+    <mergeCell ref="B61:K61"/>
+    <mergeCell ref="B55:K55"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="D56:E56"/>
+    <mergeCell ref="F56:I56"/>
+    <mergeCell ref="J56:K56"/>
+    <mergeCell ref="B60:C60"/>
+    <mergeCell ref="D60:E60"/>
+    <mergeCell ref="F60:I60"/>
+    <mergeCell ref="J60:K60"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="D59:E59"/>
+    <mergeCell ref="D40:I40"/>
+    <mergeCell ref="D41:I41"/>
+    <mergeCell ref="B42:K42"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="G37:H37"/>
+    <mergeCell ref="D37:F37"/>
+    <mergeCell ref="I37:K37"/>
+    <mergeCell ref="B38:K38"/>
+    <mergeCell ref="B39:K39"/>
+    <mergeCell ref="B2:K2"/>
+    <mergeCell ref="B3:K3"/>
+    <mergeCell ref="B4:K28"/>
+    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="E29:K29"/>
+    <mergeCell ref="B94:K94"/>
+    <mergeCell ref="B95:K95"/>
+    <mergeCell ref="B96:K99"/>
+    <mergeCell ref="B100:C100"/>
+    <mergeCell ref="D100:F100"/>
+    <mergeCell ref="G100:H100"/>
+    <mergeCell ref="I100:K100"/>
+    <mergeCell ref="B33:K36"/>
+    <mergeCell ref="B52:K52"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="F43:I43"/>
+    <mergeCell ref="J43:K43"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="F45:I45"/>
+    <mergeCell ref="J45:K45"/>
+    <mergeCell ref="B46:K46"/>
+    <mergeCell ref="B47:K50"/>
+    <mergeCell ref="B112:K112"/>
+    <mergeCell ref="B113:K113"/>
+    <mergeCell ref="B114:C114"/>
+    <mergeCell ref="D114:I114"/>
+    <mergeCell ref="J114:K114"/>
+    <mergeCell ref="B115:C115"/>
+    <mergeCell ref="D115:I115"/>
+    <mergeCell ref="J115:K115"/>
+    <mergeCell ref="B101:K101"/>
+    <mergeCell ref="B102:K102"/>
+    <mergeCell ref="B103:C103"/>
+    <mergeCell ref="D103:I103"/>
+    <mergeCell ref="J103:K103"/>
+    <mergeCell ref="B104:K104"/>
+    <mergeCell ref="B105:C105"/>
+    <mergeCell ref="D105:E105"/>
+    <mergeCell ref="F105:I105"/>
+    <mergeCell ref="J105:K105"/>
+    <mergeCell ref="B120:K120"/>
+    <mergeCell ref="B121:K121"/>
+    <mergeCell ref="B106:C106"/>
+    <mergeCell ref="D106:E106"/>
+    <mergeCell ref="J106:K106"/>
+    <mergeCell ref="F106:I106"/>
+    <mergeCell ref="B123:K123"/>
+    <mergeCell ref="B124:K124"/>
+    <mergeCell ref="B125:K128"/>
+    <mergeCell ref="B119:C119"/>
+    <mergeCell ref="D119:E119"/>
+    <mergeCell ref="F119:I119"/>
+    <mergeCell ref="J119:K119"/>
+    <mergeCell ref="B116:K116"/>
+    <mergeCell ref="B117:C117"/>
+    <mergeCell ref="D117:E117"/>
+    <mergeCell ref="F117:I117"/>
+    <mergeCell ref="J117:K117"/>
+    <mergeCell ref="B118:C118"/>
+    <mergeCell ref="D118:E118"/>
+    <mergeCell ref="F118:I118"/>
+    <mergeCell ref="J118:K118"/>
+    <mergeCell ref="B107:K107"/>
+    <mergeCell ref="B108:K111"/>
+    <mergeCell ref="B129:C129"/>
+    <mergeCell ref="D129:F129"/>
+    <mergeCell ref="G129:H129"/>
+    <mergeCell ref="I129:K129"/>
+    <mergeCell ref="B130:K130"/>
+    <mergeCell ref="B131:K131"/>
+    <mergeCell ref="B132:C132"/>
+    <mergeCell ref="D132:I132"/>
+    <mergeCell ref="J132:K132"/>
+    <mergeCell ref="B133:K133"/>
+    <mergeCell ref="B134:C134"/>
+    <mergeCell ref="D134:E134"/>
+    <mergeCell ref="F134:I134"/>
+    <mergeCell ref="J134:K134"/>
+    <mergeCell ref="B135:C135"/>
+    <mergeCell ref="D135:E135"/>
+    <mergeCell ref="F135:I135"/>
+    <mergeCell ref="J135:K135"/>
+    <mergeCell ref="B136:K136"/>
+    <mergeCell ref="B137:K140"/>
+    <mergeCell ref="B141:K141"/>
+    <mergeCell ref="B142:K142"/>
+    <mergeCell ref="B143:C143"/>
+    <mergeCell ref="D143:I143"/>
+    <mergeCell ref="J143:K143"/>
+    <mergeCell ref="B144:C144"/>
+    <mergeCell ref="D144:I144"/>
+    <mergeCell ref="J144:K144"/>
+    <mergeCell ref="B148:C148"/>
+    <mergeCell ref="D148:E148"/>
+    <mergeCell ref="F148:I148"/>
+    <mergeCell ref="J148:K148"/>
+    <mergeCell ref="B149:K149"/>
+    <mergeCell ref="B150:K150"/>
+    <mergeCell ref="B145:K145"/>
+    <mergeCell ref="B146:C146"/>
+    <mergeCell ref="D146:E146"/>
+    <mergeCell ref="F146:I146"/>
+    <mergeCell ref="J146:K146"/>
+    <mergeCell ref="B147:C147"/>
+    <mergeCell ref="D147:E147"/>
+    <mergeCell ref="F147:I147"/>
+    <mergeCell ref="J147:K147"/>
+    <mergeCell ref="B182:K182"/>
+    <mergeCell ref="B183:K183"/>
+    <mergeCell ref="B184:K187"/>
+    <mergeCell ref="B188:C188"/>
+    <mergeCell ref="D188:F188"/>
+    <mergeCell ref="G188:H188"/>
+    <mergeCell ref="I188:K188"/>
+    <mergeCell ref="B189:K189"/>
+    <mergeCell ref="B190:K190"/>
+    <mergeCell ref="B191:C191"/>
+    <mergeCell ref="D191:I191"/>
+    <mergeCell ref="J191:K191"/>
+    <mergeCell ref="B192:K192"/>
+    <mergeCell ref="B193:C193"/>
+    <mergeCell ref="D193:E193"/>
+    <mergeCell ref="F193:I193"/>
+    <mergeCell ref="J193:K193"/>
+    <mergeCell ref="B194:C194"/>
+    <mergeCell ref="D194:E194"/>
+    <mergeCell ref="F194:I194"/>
+    <mergeCell ref="J194:K194"/>
     <mergeCell ref="B212:K212"/>
     <mergeCell ref="B196:C196"/>
     <mergeCell ref="D196:E196"/>
@@ -4837,289 +5107,19 @@
     <mergeCell ref="B198:K198"/>
     <mergeCell ref="B199:K202"/>
     <mergeCell ref="B203:K203"/>
+    <mergeCell ref="B195:C195"/>
+    <mergeCell ref="D195:E195"/>
+    <mergeCell ref="F195:I195"/>
+    <mergeCell ref="J195:K195"/>
+    <mergeCell ref="B210:C210"/>
+    <mergeCell ref="D210:E210"/>
+    <mergeCell ref="F210:I210"/>
+    <mergeCell ref="J210:K210"/>
+    <mergeCell ref="B211:K211"/>
     <mergeCell ref="B204:K204"/>
     <mergeCell ref="B205:C205"/>
     <mergeCell ref="D205:I205"/>
     <mergeCell ref="J205:K205"/>
-    <mergeCell ref="B191:C191"/>
-    <mergeCell ref="D191:I191"/>
-    <mergeCell ref="J191:K191"/>
-    <mergeCell ref="B192:K192"/>
-    <mergeCell ref="B193:C193"/>
-    <mergeCell ref="D193:E193"/>
-    <mergeCell ref="F193:I193"/>
-    <mergeCell ref="J193:K193"/>
-    <mergeCell ref="B194:C194"/>
-    <mergeCell ref="D194:E194"/>
-    <mergeCell ref="F194:I194"/>
-    <mergeCell ref="J194:K194"/>
-    <mergeCell ref="B182:K182"/>
-    <mergeCell ref="B183:K183"/>
-    <mergeCell ref="B184:K187"/>
-    <mergeCell ref="B188:C188"/>
-    <mergeCell ref="D188:F188"/>
-    <mergeCell ref="G188:H188"/>
-    <mergeCell ref="I188:K188"/>
-    <mergeCell ref="B189:K189"/>
-    <mergeCell ref="B190:K190"/>
-    <mergeCell ref="B148:C148"/>
-    <mergeCell ref="D148:E148"/>
-    <mergeCell ref="F148:I148"/>
-    <mergeCell ref="J148:K148"/>
-    <mergeCell ref="B149:K149"/>
-    <mergeCell ref="B150:K150"/>
-    <mergeCell ref="B145:K145"/>
-    <mergeCell ref="B146:C146"/>
-    <mergeCell ref="D146:E146"/>
-    <mergeCell ref="F146:I146"/>
-    <mergeCell ref="J146:K146"/>
-    <mergeCell ref="B147:C147"/>
-    <mergeCell ref="D147:E147"/>
-    <mergeCell ref="F147:I147"/>
-    <mergeCell ref="J147:K147"/>
-    <mergeCell ref="B136:K136"/>
-    <mergeCell ref="B137:K140"/>
-    <mergeCell ref="B141:K141"/>
-    <mergeCell ref="B142:K142"/>
-    <mergeCell ref="B143:C143"/>
-    <mergeCell ref="D143:I143"/>
-    <mergeCell ref="J143:K143"/>
-    <mergeCell ref="B144:C144"/>
-    <mergeCell ref="D144:I144"/>
-    <mergeCell ref="J144:K144"/>
-    <mergeCell ref="B133:K133"/>
-    <mergeCell ref="B134:C134"/>
-    <mergeCell ref="D134:E134"/>
-    <mergeCell ref="F134:I134"/>
-    <mergeCell ref="J134:K134"/>
-    <mergeCell ref="B135:C135"/>
-    <mergeCell ref="D135:E135"/>
-    <mergeCell ref="F135:I135"/>
-    <mergeCell ref="J135:K135"/>
-    <mergeCell ref="B129:C129"/>
-    <mergeCell ref="D129:F129"/>
-    <mergeCell ref="G129:H129"/>
-    <mergeCell ref="I129:K129"/>
-    <mergeCell ref="B130:K130"/>
-    <mergeCell ref="B131:K131"/>
-    <mergeCell ref="B132:C132"/>
-    <mergeCell ref="D132:I132"/>
-    <mergeCell ref="J132:K132"/>
-    <mergeCell ref="B120:K120"/>
-    <mergeCell ref="B121:K121"/>
-    <mergeCell ref="B106:C106"/>
-    <mergeCell ref="D106:E106"/>
-    <mergeCell ref="J106:K106"/>
-    <mergeCell ref="F106:I106"/>
-    <mergeCell ref="B123:K123"/>
-    <mergeCell ref="B124:K124"/>
-    <mergeCell ref="B125:K128"/>
-    <mergeCell ref="B119:C119"/>
-    <mergeCell ref="D119:E119"/>
-    <mergeCell ref="F119:I119"/>
-    <mergeCell ref="J119:K119"/>
-    <mergeCell ref="B116:K116"/>
-    <mergeCell ref="B117:C117"/>
-    <mergeCell ref="D117:E117"/>
-    <mergeCell ref="F117:I117"/>
-    <mergeCell ref="J117:K117"/>
-    <mergeCell ref="B118:C118"/>
-    <mergeCell ref="D118:E118"/>
-    <mergeCell ref="F118:I118"/>
-    <mergeCell ref="J118:K118"/>
-    <mergeCell ref="B107:K107"/>
-    <mergeCell ref="B108:K111"/>
-    <mergeCell ref="B112:K112"/>
-    <mergeCell ref="B113:K113"/>
-    <mergeCell ref="B114:C114"/>
-    <mergeCell ref="D114:I114"/>
-    <mergeCell ref="J114:K114"/>
-    <mergeCell ref="B115:C115"/>
-    <mergeCell ref="D115:I115"/>
-    <mergeCell ref="J115:K115"/>
-    <mergeCell ref="B101:K101"/>
-    <mergeCell ref="B102:K102"/>
-    <mergeCell ref="B103:C103"/>
-    <mergeCell ref="D103:I103"/>
-    <mergeCell ref="J103:K103"/>
-    <mergeCell ref="B104:K104"/>
-    <mergeCell ref="B105:C105"/>
-    <mergeCell ref="D105:E105"/>
-    <mergeCell ref="F105:I105"/>
-    <mergeCell ref="J105:K105"/>
-    <mergeCell ref="B2:K2"/>
-    <mergeCell ref="B3:K3"/>
-    <mergeCell ref="B4:K28"/>
-    <mergeCell ref="B29:D29"/>
-    <mergeCell ref="E29:K29"/>
-    <mergeCell ref="B94:K94"/>
-    <mergeCell ref="B95:K95"/>
-    <mergeCell ref="B96:K99"/>
-    <mergeCell ref="B100:C100"/>
-    <mergeCell ref="D100:F100"/>
-    <mergeCell ref="G100:H100"/>
-    <mergeCell ref="I100:K100"/>
-    <mergeCell ref="B33:K36"/>
-    <mergeCell ref="B52:K52"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="F43:I43"/>
-    <mergeCell ref="J43:K43"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="F45:I45"/>
-    <mergeCell ref="J45:K45"/>
-    <mergeCell ref="B46:K46"/>
-    <mergeCell ref="B47:K50"/>
-    <mergeCell ref="D40:I40"/>
-    <mergeCell ref="D41:I41"/>
-    <mergeCell ref="B42:K42"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="G37:H37"/>
-    <mergeCell ref="D37:F37"/>
-    <mergeCell ref="I37:K37"/>
-    <mergeCell ref="B38:K38"/>
-    <mergeCell ref="B39:K39"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="D54:I54"/>
-    <mergeCell ref="J54:K54"/>
-    <mergeCell ref="B61:K61"/>
-    <mergeCell ref="B55:K55"/>
-    <mergeCell ref="B56:C56"/>
-    <mergeCell ref="D56:E56"/>
-    <mergeCell ref="F56:I56"/>
-    <mergeCell ref="J56:K56"/>
-    <mergeCell ref="B60:C60"/>
-    <mergeCell ref="D60:E60"/>
-    <mergeCell ref="F60:I60"/>
-    <mergeCell ref="J60:K60"/>
-    <mergeCell ref="B59:C59"/>
-    <mergeCell ref="D59:E59"/>
-    <mergeCell ref="B65:K65"/>
-    <mergeCell ref="B66:K69"/>
-    <mergeCell ref="B70:C70"/>
-    <mergeCell ref="D70:F70"/>
-    <mergeCell ref="G70:H70"/>
-    <mergeCell ref="I70:K70"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="D57:E57"/>
-    <mergeCell ref="F57:I57"/>
-    <mergeCell ref="J57:K57"/>
-    <mergeCell ref="B62:K62"/>
-    <mergeCell ref="F59:I59"/>
-    <mergeCell ref="J59:K59"/>
-    <mergeCell ref="B58:C58"/>
-    <mergeCell ref="D58:E58"/>
-    <mergeCell ref="F58:I58"/>
-    <mergeCell ref="J58:K58"/>
-    <mergeCell ref="B31:K31"/>
-    <mergeCell ref="B32:K32"/>
-    <mergeCell ref="B74:K74"/>
-    <mergeCell ref="B75:C75"/>
-    <mergeCell ref="D75:E75"/>
-    <mergeCell ref="F75:I75"/>
-    <mergeCell ref="J75:K75"/>
-    <mergeCell ref="B71:K71"/>
-    <mergeCell ref="B72:K72"/>
-    <mergeCell ref="B73:C73"/>
-    <mergeCell ref="D73:I73"/>
-    <mergeCell ref="J73:K73"/>
-    <mergeCell ref="B51:K51"/>
-    <mergeCell ref="J40:K40"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="J41:K41"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="D53:I53"/>
-    <mergeCell ref="J53:K53"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="F44:I44"/>
-    <mergeCell ref="J44:K44"/>
-    <mergeCell ref="B64:K64"/>
-    <mergeCell ref="B76:K76"/>
-    <mergeCell ref="B77:K80"/>
-    <mergeCell ref="B81:K81"/>
-    <mergeCell ref="B82:K82"/>
-    <mergeCell ref="B83:C83"/>
-    <mergeCell ref="D83:I83"/>
-    <mergeCell ref="J83:K83"/>
-    <mergeCell ref="B87:C87"/>
-    <mergeCell ref="D87:E87"/>
-    <mergeCell ref="F87:I87"/>
-    <mergeCell ref="J87:K87"/>
-    <mergeCell ref="B88:C88"/>
-    <mergeCell ref="D88:E88"/>
-    <mergeCell ref="F88:I88"/>
-    <mergeCell ref="J88:K88"/>
-    <mergeCell ref="B84:C84"/>
-    <mergeCell ref="D84:I84"/>
-    <mergeCell ref="J84:K84"/>
-    <mergeCell ref="B85:K85"/>
-    <mergeCell ref="B86:C86"/>
-    <mergeCell ref="D86:E86"/>
-    <mergeCell ref="F86:I86"/>
-    <mergeCell ref="J86:K86"/>
-    <mergeCell ref="B91:K91"/>
-    <mergeCell ref="B92:K92"/>
-    <mergeCell ref="B89:C89"/>
-    <mergeCell ref="D89:E89"/>
-    <mergeCell ref="F89:I89"/>
-    <mergeCell ref="J89:K89"/>
-    <mergeCell ref="B90:C90"/>
-    <mergeCell ref="D90:E90"/>
-    <mergeCell ref="F90:I90"/>
-    <mergeCell ref="J90:K90"/>
-    <mergeCell ref="B152:K152"/>
-    <mergeCell ref="B153:K153"/>
-    <mergeCell ref="B154:K157"/>
-    <mergeCell ref="B158:C158"/>
-    <mergeCell ref="D158:F158"/>
-    <mergeCell ref="G158:H158"/>
-    <mergeCell ref="I158:K158"/>
-    <mergeCell ref="B159:K159"/>
-    <mergeCell ref="B160:K160"/>
-    <mergeCell ref="D173:I173"/>
-    <mergeCell ref="J173:K173"/>
-    <mergeCell ref="B174:C174"/>
-    <mergeCell ref="D174:I174"/>
-    <mergeCell ref="J174:K174"/>
-    <mergeCell ref="B161:C161"/>
-    <mergeCell ref="D161:I161"/>
-    <mergeCell ref="J161:K161"/>
-    <mergeCell ref="B162:K162"/>
-    <mergeCell ref="B163:C163"/>
-    <mergeCell ref="D163:E163"/>
-    <mergeCell ref="F163:I163"/>
-    <mergeCell ref="J163:K163"/>
-    <mergeCell ref="B164:C164"/>
-    <mergeCell ref="D164:E164"/>
-    <mergeCell ref="F164:I164"/>
-    <mergeCell ref="J164:K164"/>
-    <mergeCell ref="B178:C178"/>
-    <mergeCell ref="D178:E178"/>
-    <mergeCell ref="F178:I178"/>
-    <mergeCell ref="J178:K178"/>
-    <mergeCell ref="B179:K179"/>
-    <mergeCell ref="B180:K180"/>
-    <mergeCell ref="B165:C165"/>
-    <mergeCell ref="D165:E165"/>
-    <mergeCell ref="F165:I165"/>
-    <mergeCell ref="J165:K165"/>
-    <mergeCell ref="B175:K175"/>
-    <mergeCell ref="B176:C176"/>
-    <mergeCell ref="D176:E176"/>
-    <mergeCell ref="F176:I176"/>
-    <mergeCell ref="J176:K176"/>
-    <mergeCell ref="B177:C177"/>
-    <mergeCell ref="D177:E177"/>
-    <mergeCell ref="F177:I177"/>
-    <mergeCell ref="J177:K177"/>
-    <mergeCell ref="B166:K166"/>
-    <mergeCell ref="B167:K170"/>
-    <mergeCell ref="B171:K171"/>
-    <mergeCell ref="B172:K172"/>
-    <mergeCell ref="B173:C173"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>